<commit_message>
KeyAssign: add graphic to pinmap.xls
</commit_message>
<xml_diff>
--- a/PolysixKeyAssigner/KeyAssignerPinMap - Arduino Mega 2560.xlsx
+++ b/PolysixKeyAssigner/KeyAssignerPinMap - Arduino Mega 2560.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="195">
   <si>
     <t>Pin Number</t>
   </si>
@@ -601,6 +601,9 @@
   </si>
   <si>
     <t>I2C SCL to DAC</t>
+  </si>
+  <si>
+    <t>Input (Pullup)</t>
   </si>
 </sst>
 </file>
@@ -697,12 +700,1914 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF00FF00"/>
+      <color rgb="FF008000"/>
+      <color rgb="FF00CC00"/>
+      <color rgb="FF0000FF"/>
+      <color rgb="FF00FFFF"/>
+      <color rgb="FFFF00FF"/>
+      <color rgb="FFCC00CC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>326517</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>11903</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>22801</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>19843</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="62" name="Group 61"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="7744111" y="2881309"/>
+          <a:ext cx="4923128" cy="2341565"/>
+          <a:chOff x="8006049" y="10548935"/>
+          <a:chExt cx="4875503" cy="2341565"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="2" name="Picture 1" descr="http://flipmu.com/files/2011/12/ArduinoMega2650Front_21.jpg"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill rotWithShape="1">
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect t="5948" r="4153" b="9875"/>
+          <a:stretch/>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm rot="10800000">
+            <a:off x="8006049" y="10548935"/>
+            <a:ext cx="4875503" cy="2341565"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="3" name="Oval 2"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="9815802" y="12668249"/>
+            <a:ext cx="124476" cy="127722"/>
+          </a:xfrm>
+          <a:prstGeom prst="ellipse">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="00FF00"/>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="4" name="Oval 3"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="9911052" y="12668249"/>
+            <a:ext cx="124476" cy="127722"/>
+          </a:xfrm>
+          <a:prstGeom prst="ellipse">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="00FF00"/>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="5" name="Oval 4"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="10023620" y="12668249"/>
+            <a:ext cx="124476" cy="127722"/>
+          </a:xfrm>
+          <a:prstGeom prst="ellipse">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="00FF00"/>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="6" name="Oval 5"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="9261260" y="12668249"/>
+            <a:ext cx="124476" cy="127722"/>
+          </a:xfrm>
+          <a:prstGeom prst="ellipse">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="FFFF00"/>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="7" name="Oval 6"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="9140754" y="12668249"/>
+            <a:ext cx="124476" cy="127722"/>
+          </a:xfrm>
+          <a:prstGeom prst="ellipse">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="FFFF00"/>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="8" name="Oval 7"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="8924998" y="12668249"/>
+            <a:ext cx="124476" cy="127722"/>
+          </a:xfrm>
+          <a:prstGeom prst="ellipse">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="00FF00"/>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="9" name="Oval 8"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="8821088" y="12668249"/>
+            <a:ext cx="124476" cy="127722"/>
+          </a:xfrm>
+          <a:prstGeom prst="ellipse">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="00FF00"/>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="10" name="Oval 9"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="8708520" y="12668249"/>
+            <a:ext cx="124476" cy="127722"/>
+          </a:xfrm>
+          <a:prstGeom prst="ellipse">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="0000FF"/>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="11" name="Oval 10"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="8612549" y="12668249"/>
+            <a:ext cx="124476" cy="127722"/>
+          </a:xfrm>
+          <a:prstGeom prst="ellipse">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="0000FF"/>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="31" name="Group 30"/>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="8162997" y="12256634"/>
+            <a:ext cx="215601" cy="421358"/>
+            <a:chOff x="8238970" y="9493250"/>
+            <a:chExt cx="215601" cy="427028"/>
+          </a:xfrm>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </xdr:grpSpPr>
+        <xdr:grpSp>
+          <xdr:nvGrpSpPr>
+            <xdr:cNvPr id="21" name="Group 20"/>
+            <xdr:cNvGrpSpPr/>
+          </xdr:nvGrpSpPr>
+          <xdr:grpSpPr>
+            <a:xfrm>
+              <a:off x="8238970" y="9493250"/>
+              <a:ext cx="215601" cy="109527"/>
+              <a:chOff x="8238970" y="9493250"/>
+              <a:chExt cx="215601" cy="109527"/>
+            </a:xfrm>
+            <a:grpFill/>
+          </xdr:grpSpPr>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="19" name="Oval 18"/>
+              <xdr:cNvSpPr/>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="8238970" y="9493250"/>
+                <a:ext cx="111280" cy="109527"/>
+              </a:xfrm>
+              <a:prstGeom prst="ellipse">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:grpFill/>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="2">
+                <a:schemeClr val="accent1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:lnRef>
+              <a:fillRef idx="1">
+                <a:schemeClr val="accent1"/>
+              </a:fillRef>
+              <a:effectRef idx="0">
+                <a:schemeClr val="accent1"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="lt1"/>
+              </a:fontRef>
+            </xdr:style>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="l"/>
+                <a:endParaRPr lang="en-US" sz="1100"/>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="20" name="Oval 19"/>
+              <xdr:cNvSpPr/>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="8343291" y="9493250"/>
+                <a:ext cx="111280" cy="109527"/>
+              </a:xfrm>
+              <a:prstGeom prst="ellipse">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:grpFill/>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="2">
+                <a:schemeClr val="accent1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:lnRef>
+              <a:fillRef idx="1">
+                <a:schemeClr val="accent1"/>
+              </a:fillRef>
+              <a:effectRef idx="0">
+                <a:schemeClr val="accent1"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="lt1"/>
+              </a:fontRef>
+            </xdr:style>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="l"/>
+                <a:endParaRPr lang="en-US" sz="1100"/>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+        </xdr:grpSp>
+        <xdr:grpSp>
+          <xdr:nvGrpSpPr>
+            <xdr:cNvPr id="22" name="Group 21"/>
+            <xdr:cNvGrpSpPr/>
+          </xdr:nvGrpSpPr>
+          <xdr:grpSpPr>
+            <a:xfrm>
+              <a:off x="8238970" y="9599084"/>
+              <a:ext cx="215601" cy="109527"/>
+              <a:chOff x="8238970" y="9493250"/>
+              <a:chExt cx="215601" cy="109527"/>
+            </a:xfrm>
+            <a:grpFill/>
+          </xdr:grpSpPr>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="23" name="Oval 22"/>
+              <xdr:cNvSpPr/>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="8238970" y="9493250"/>
+                <a:ext cx="111280" cy="109527"/>
+              </a:xfrm>
+              <a:prstGeom prst="ellipse">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:grpFill/>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="2">
+                <a:schemeClr val="accent1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:lnRef>
+              <a:fillRef idx="1">
+                <a:schemeClr val="accent1"/>
+              </a:fillRef>
+              <a:effectRef idx="0">
+                <a:schemeClr val="accent1"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="lt1"/>
+              </a:fontRef>
+            </xdr:style>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="l"/>
+                <a:endParaRPr lang="en-US" sz="1100"/>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="24" name="Oval 23"/>
+              <xdr:cNvSpPr/>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="8343291" y="9493250"/>
+                <a:ext cx="111280" cy="109527"/>
+              </a:xfrm>
+              <a:prstGeom prst="ellipse">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:grpFill/>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="2">
+                <a:schemeClr val="accent1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:lnRef>
+              <a:fillRef idx="1">
+                <a:schemeClr val="accent1"/>
+              </a:fillRef>
+              <a:effectRef idx="0">
+                <a:schemeClr val="accent1"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="lt1"/>
+              </a:fontRef>
+            </xdr:style>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="l"/>
+                <a:endParaRPr lang="en-US" sz="1100"/>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+        </xdr:grpSp>
+        <xdr:grpSp>
+          <xdr:nvGrpSpPr>
+            <xdr:cNvPr id="25" name="Group 24"/>
+            <xdr:cNvGrpSpPr/>
+          </xdr:nvGrpSpPr>
+          <xdr:grpSpPr>
+            <a:xfrm>
+              <a:off x="8238970" y="9704918"/>
+              <a:ext cx="215601" cy="109527"/>
+              <a:chOff x="8238970" y="9493250"/>
+              <a:chExt cx="215601" cy="109527"/>
+            </a:xfrm>
+            <a:grpFill/>
+          </xdr:grpSpPr>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="26" name="Oval 25"/>
+              <xdr:cNvSpPr/>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="8238970" y="9493250"/>
+                <a:ext cx="111280" cy="109527"/>
+              </a:xfrm>
+              <a:prstGeom prst="ellipse">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:grpFill/>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="2">
+                <a:schemeClr val="accent1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:lnRef>
+              <a:fillRef idx="1">
+                <a:schemeClr val="accent1"/>
+              </a:fillRef>
+              <a:effectRef idx="0">
+                <a:schemeClr val="accent1"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="lt1"/>
+              </a:fontRef>
+            </xdr:style>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="l"/>
+                <a:endParaRPr lang="en-US" sz="1100"/>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="27" name="Oval 26"/>
+              <xdr:cNvSpPr/>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="8343291" y="9493250"/>
+                <a:ext cx="111280" cy="109527"/>
+              </a:xfrm>
+              <a:prstGeom prst="ellipse">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:grpFill/>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="2">
+                <a:schemeClr val="accent1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:lnRef>
+              <a:fillRef idx="1">
+                <a:schemeClr val="accent1"/>
+              </a:fillRef>
+              <a:effectRef idx="0">
+                <a:schemeClr val="accent1"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="lt1"/>
+              </a:fontRef>
+            </xdr:style>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="l"/>
+                <a:endParaRPr lang="en-US" sz="1100"/>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+        </xdr:grpSp>
+        <xdr:grpSp>
+          <xdr:nvGrpSpPr>
+            <xdr:cNvPr id="28" name="Group 27"/>
+            <xdr:cNvGrpSpPr/>
+          </xdr:nvGrpSpPr>
+          <xdr:grpSpPr>
+            <a:xfrm>
+              <a:off x="8238970" y="9810751"/>
+              <a:ext cx="215601" cy="109527"/>
+              <a:chOff x="8238970" y="9493250"/>
+              <a:chExt cx="215601" cy="109527"/>
+            </a:xfrm>
+            <a:grpFill/>
+          </xdr:grpSpPr>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="29" name="Oval 28"/>
+              <xdr:cNvSpPr/>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="8238970" y="9493250"/>
+                <a:ext cx="111280" cy="109527"/>
+              </a:xfrm>
+              <a:prstGeom prst="ellipse">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:grpFill/>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="2">
+                <a:schemeClr val="accent1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:lnRef>
+              <a:fillRef idx="1">
+                <a:schemeClr val="accent1"/>
+              </a:fillRef>
+              <a:effectRef idx="0">
+                <a:schemeClr val="accent1"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="lt1"/>
+              </a:fontRef>
+            </xdr:style>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="l"/>
+                <a:endParaRPr lang="en-US" sz="1100"/>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="30" name="Oval 29"/>
+              <xdr:cNvSpPr/>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="8343291" y="9493250"/>
+                <a:ext cx="111280" cy="109527"/>
+              </a:xfrm>
+              <a:prstGeom prst="ellipse">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:grpFill/>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="2">
+                <a:schemeClr val="accent1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:lnRef>
+              <a:fillRef idx="1">
+                <a:schemeClr val="accent1"/>
+              </a:fillRef>
+              <a:effectRef idx="0">
+                <a:schemeClr val="accent1"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="lt1"/>
+              </a:fontRef>
+            </xdr:style>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="l"/>
+                <a:endParaRPr lang="en-US" sz="1100"/>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+        </xdr:grpSp>
+      </xdr:grpSp>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="32" name="Group 31"/>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="8162997" y="11825741"/>
+            <a:ext cx="215601" cy="422492"/>
+            <a:chOff x="8238970" y="9493250"/>
+            <a:chExt cx="215601" cy="427028"/>
+          </a:xfrm>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </xdr:grpSpPr>
+        <xdr:grpSp>
+          <xdr:nvGrpSpPr>
+            <xdr:cNvPr id="33" name="Group 32"/>
+            <xdr:cNvGrpSpPr/>
+          </xdr:nvGrpSpPr>
+          <xdr:grpSpPr>
+            <a:xfrm>
+              <a:off x="8238970" y="9493250"/>
+              <a:ext cx="215601" cy="109527"/>
+              <a:chOff x="8238970" y="9493250"/>
+              <a:chExt cx="215601" cy="109527"/>
+            </a:xfrm>
+            <a:grpFill/>
+          </xdr:grpSpPr>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="43" name="Oval 42"/>
+              <xdr:cNvSpPr/>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="8238970" y="9493250"/>
+                <a:ext cx="111280" cy="109527"/>
+              </a:xfrm>
+              <a:prstGeom prst="ellipse">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:grpFill/>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="2">
+                <a:schemeClr val="accent1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:lnRef>
+              <a:fillRef idx="1">
+                <a:schemeClr val="accent1"/>
+              </a:fillRef>
+              <a:effectRef idx="0">
+                <a:schemeClr val="accent1"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="lt1"/>
+              </a:fontRef>
+            </xdr:style>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="l"/>
+                <a:endParaRPr lang="en-US" sz="1100"/>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="44" name="Oval 43"/>
+              <xdr:cNvSpPr/>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="8343291" y="9493250"/>
+                <a:ext cx="111280" cy="109527"/>
+              </a:xfrm>
+              <a:prstGeom prst="ellipse">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:grpFill/>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="2">
+                <a:schemeClr val="accent1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:lnRef>
+              <a:fillRef idx="1">
+                <a:schemeClr val="accent1"/>
+              </a:fillRef>
+              <a:effectRef idx="0">
+                <a:schemeClr val="accent1"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="lt1"/>
+              </a:fontRef>
+            </xdr:style>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="l"/>
+                <a:endParaRPr lang="en-US" sz="1100"/>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+        </xdr:grpSp>
+        <xdr:grpSp>
+          <xdr:nvGrpSpPr>
+            <xdr:cNvPr id="34" name="Group 33"/>
+            <xdr:cNvGrpSpPr/>
+          </xdr:nvGrpSpPr>
+          <xdr:grpSpPr>
+            <a:xfrm>
+              <a:off x="8238970" y="9599084"/>
+              <a:ext cx="215601" cy="109527"/>
+              <a:chOff x="8238970" y="9493250"/>
+              <a:chExt cx="215601" cy="109527"/>
+            </a:xfrm>
+            <a:grpFill/>
+          </xdr:grpSpPr>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="41" name="Oval 40"/>
+              <xdr:cNvSpPr/>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="8238970" y="9493250"/>
+                <a:ext cx="111280" cy="109527"/>
+              </a:xfrm>
+              <a:prstGeom prst="ellipse">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:grpFill/>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="2">
+                <a:schemeClr val="accent1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:lnRef>
+              <a:fillRef idx="1">
+                <a:schemeClr val="accent1"/>
+              </a:fillRef>
+              <a:effectRef idx="0">
+                <a:schemeClr val="accent1"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="lt1"/>
+              </a:fontRef>
+            </xdr:style>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="l"/>
+                <a:endParaRPr lang="en-US" sz="1100"/>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="42" name="Oval 41"/>
+              <xdr:cNvSpPr/>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="8343291" y="9493250"/>
+                <a:ext cx="111280" cy="109527"/>
+              </a:xfrm>
+              <a:prstGeom prst="ellipse">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:grpFill/>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="2">
+                <a:schemeClr val="accent1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:lnRef>
+              <a:fillRef idx="1">
+                <a:schemeClr val="accent1"/>
+              </a:fillRef>
+              <a:effectRef idx="0">
+                <a:schemeClr val="accent1"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="lt1"/>
+              </a:fontRef>
+            </xdr:style>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="l"/>
+                <a:endParaRPr lang="en-US" sz="1100"/>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+        </xdr:grpSp>
+        <xdr:grpSp>
+          <xdr:nvGrpSpPr>
+            <xdr:cNvPr id="35" name="Group 34"/>
+            <xdr:cNvGrpSpPr/>
+          </xdr:nvGrpSpPr>
+          <xdr:grpSpPr>
+            <a:xfrm>
+              <a:off x="8238970" y="9704918"/>
+              <a:ext cx="215601" cy="109527"/>
+              <a:chOff x="8238970" y="9493250"/>
+              <a:chExt cx="215601" cy="109527"/>
+            </a:xfrm>
+            <a:grpFill/>
+          </xdr:grpSpPr>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="39" name="Oval 38"/>
+              <xdr:cNvSpPr/>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="8238970" y="9493250"/>
+                <a:ext cx="111280" cy="109527"/>
+              </a:xfrm>
+              <a:prstGeom prst="ellipse">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:grpFill/>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="2">
+                <a:schemeClr val="accent1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:lnRef>
+              <a:fillRef idx="1">
+                <a:schemeClr val="accent1"/>
+              </a:fillRef>
+              <a:effectRef idx="0">
+                <a:schemeClr val="accent1"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="lt1"/>
+              </a:fontRef>
+            </xdr:style>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="l"/>
+                <a:endParaRPr lang="en-US" sz="1100"/>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="40" name="Oval 39"/>
+              <xdr:cNvSpPr/>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="8343291" y="9493250"/>
+                <a:ext cx="111280" cy="109527"/>
+              </a:xfrm>
+              <a:prstGeom prst="ellipse">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:grpFill/>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="2">
+                <a:schemeClr val="accent1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:lnRef>
+              <a:fillRef idx="1">
+                <a:schemeClr val="accent1"/>
+              </a:fillRef>
+              <a:effectRef idx="0">
+                <a:schemeClr val="accent1"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="lt1"/>
+              </a:fontRef>
+            </xdr:style>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="l"/>
+                <a:endParaRPr lang="en-US" sz="1100"/>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+        </xdr:grpSp>
+        <xdr:grpSp>
+          <xdr:nvGrpSpPr>
+            <xdr:cNvPr id="36" name="Group 35"/>
+            <xdr:cNvGrpSpPr/>
+          </xdr:nvGrpSpPr>
+          <xdr:grpSpPr>
+            <a:xfrm>
+              <a:off x="8238970" y="9810751"/>
+              <a:ext cx="215601" cy="109527"/>
+              <a:chOff x="8238970" y="9493250"/>
+              <a:chExt cx="215601" cy="109527"/>
+            </a:xfrm>
+            <a:grpFill/>
+          </xdr:grpSpPr>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="37" name="Oval 36"/>
+              <xdr:cNvSpPr/>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="8238970" y="9493250"/>
+                <a:ext cx="111280" cy="109527"/>
+              </a:xfrm>
+              <a:prstGeom prst="ellipse">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:grpFill/>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="2">
+                <a:schemeClr val="accent1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:lnRef>
+              <a:fillRef idx="1">
+                <a:schemeClr val="accent1"/>
+              </a:fillRef>
+              <a:effectRef idx="0">
+                <a:schemeClr val="accent1"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="lt1"/>
+              </a:fontRef>
+            </xdr:style>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="l"/>
+                <a:endParaRPr lang="en-US" sz="1100"/>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+          <xdr:sp macro="" textlink="">
+            <xdr:nvSpPr>
+              <xdr:cNvPr id="38" name="Oval 37"/>
+              <xdr:cNvSpPr/>
+            </xdr:nvSpPr>
+            <xdr:spPr>
+              <a:xfrm>
+                <a:off x="8343291" y="9493250"/>
+                <a:ext cx="111280" cy="109527"/>
+              </a:xfrm>
+              <a:prstGeom prst="ellipse">
+                <a:avLst/>
+              </a:prstGeom>
+              <a:grpFill/>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+            </xdr:spPr>
+            <xdr:style>
+              <a:lnRef idx="2">
+                <a:schemeClr val="accent1">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
+              </a:lnRef>
+              <a:fillRef idx="1">
+                <a:schemeClr val="accent1"/>
+              </a:fillRef>
+              <a:effectRef idx="0">
+                <a:schemeClr val="accent1"/>
+              </a:effectRef>
+              <a:fontRef idx="minor">
+                <a:schemeClr val="lt1"/>
+              </a:fontRef>
+            </xdr:style>
+            <xdr:txBody>
+              <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="l"/>
+                <a:endParaRPr lang="en-US" sz="1100"/>
+              </a:p>
+            </xdr:txBody>
+          </xdr:sp>
+        </xdr:grpSp>
+      </xdr:grpSp>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="46" name="Group 45"/>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="8162997" y="11393146"/>
+            <a:ext cx="215601" cy="106431"/>
+            <a:chOff x="8238970" y="9493250"/>
+            <a:chExt cx="215601" cy="109527"/>
+          </a:xfrm>
+          <a:solidFill>
+            <a:srgbClr val="00FF00"/>
+          </a:solidFill>
+        </xdr:grpSpPr>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="56" name="Oval 55"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8238970" y="9493250"/>
+              <a:ext cx="111280" cy="109527"/>
+            </a:xfrm>
+            <a:prstGeom prst="ellipse">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:grpFill/>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="57" name="Oval 56"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8343291" y="9493250"/>
+              <a:ext cx="111280" cy="109527"/>
+            </a:xfrm>
+            <a:prstGeom prst="ellipse">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:grpFill/>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="47" name="Group 46"/>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="8162997" y="11495855"/>
+            <a:ext cx="215601" cy="110399"/>
+            <a:chOff x="8238970" y="9493250"/>
+            <a:chExt cx="215601" cy="109527"/>
+          </a:xfrm>
+          <a:solidFill>
+            <a:srgbClr val="00FF00"/>
+          </a:solidFill>
+        </xdr:grpSpPr>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="54" name="Oval 53"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8238970" y="9493250"/>
+              <a:ext cx="111280" cy="109527"/>
+            </a:xfrm>
+            <a:prstGeom prst="ellipse">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:grpFill/>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="55" name="Oval 54"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8343291" y="9493250"/>
+              <a:ext cx="111280" cy="109527"/>
+            </a:xfrm>
+            <a:prstGeom prst="ellipse">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:grpFill/>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="48" name="Group 47"/>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="8162997" y="11602532"/>
+            <a:ext cx="215601" cy="106429"/>
+            <a:chOff x="8238970" y="9493250"/>
+            <a:chExt cx="215601" cy="109527"/>
+          </a:xfrm>
+          <a:solidFill>
+            <a:srgbClr val="00FF00"/>
+          </a:solidFill>
+        </xdr:grpSpPr>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="52" name="Oval 51"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8238970" y="9493250"/>
+              <a:ext cx="111280" cy="109527"/>
+            </a:xfrm>
+            <a:prstGeom prst="ellipse">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:grpFill/>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="53" name="Oval 52"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8343291" y="9493250"/>
+              <a:ext cx="111280" cy="109527"/>
+            </a:xfrm>
+            <a:prstGeom prst="ellipse">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:grpFill/>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="49" name="Group 48"/>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="8162997" y="11705238"/>
+            <a:ext cx="215601" cy="106431"/>
+            <a:chOff x="8238970" y="9493250"/>
+            <a:chExt cx="215601" cy="109527"/>
+          </a:xfrm>
+          <a:solidFill>
+            <a:srgbClr val="00FF00"/>
+          </a:solidFill>
+        </xdr:grpSpPr>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="50" name="Oval 49"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8238970" y="9493250"/>
+              <a:ext cx="111280" cy="109527"/>
+            </a:xfrm>
+            <a:prstGeom prst="ellipse">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:grpFill/>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="51" name="Oval 50"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8343291" y="9493250"/>
+              <a:ext cx="111280" cy="109527"/>
+            </a:xfrm>
+            <a:prstGeom prst="ellipse">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:grpFill/>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="60" name="Oval 59"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="8267318" y="11282021"/>
+            <a:ext cx="111280" cy="110399"/>
+          </a:xfrm>
+          <a:prstGeom prst="ellipse">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="00FF00"/>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="61" name="Oval 60"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="8180006" y="10948646"/>
+            <a:ext cx="111280" cy="110399"/>
+          </a:xfrm>
+          <a:prstGeom prst="ellipse">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="00FF00"/>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -992,15 +2897,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:F105"/>
+  <dimension ref="B3:K105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L77" sqref="K71:L77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.28515625" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="4"/>
+    <col min="1" max="1" width="3.42578125" style="4" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" style="4" customWidth="1"/>
     <col min="3" max="3" width="29" style="4" customWidth="1"/>
     <col min="4" max="4" width="21" style="4" customWidth="1"/>
@@ -1170,7 +3075,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="2">
         <v>84</v>
       </c>
@@ -1181,7 +3086,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="2">
         <v>83</v>
       </c>
@@ -1192,7 +3097,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11" ht="15" x14ac:dyDescent="0.25">
       <c r="B19" s="2">
         <v>82</v>
       </c>
@@ -1202,8 +3107,9 @@
       <c r="D19" s="2" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="K19"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="2">
         <v>98</v>
       </c>
@@ -1214,7 +3120,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" s="2">
         <v>2</v>
       </c>
@@ -1225,7 +3131,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" s="2">
         <v>3</v>
       </c>
@@ -1236,7 +3142,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" s="2">
         <v>6</v>
       </c>
@@ -1250,10 +3156,10 @@
         <v>190</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" s="2">
         <v>7</v>
       </c>
@@ -1270,7 +3176,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" s="2">
         <v>1</v>
       </c>
@@ -1287,7 +3193,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26" s="2">
         <v>5</v>
       </c>
@@ -1298,7 +3204,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" s="2">
         <v>15</v>
       </c>
@@ -1309,7 +3215,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" s="2">
         <v>16</v>
       </c>
@@ -1320,7 +3226,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" s="2">
         <v>17</v>
       </c>
@@ -1331,7 +3237,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" s="2">
         <v>18</v>
       </c>
@@ -1342,7 +3248,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" s="2">
         <v>23</v>
       </c>
@@ -1353,7 +3259,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B32" s="2">
         <v>24</v>
       </c>
@@ -1456,7 +3362,7 @@
         <v>183</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>158</v>
+        <v>194</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
@@ -2015,7 +3921,7 @@
         <v>188</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>158</v>
+        <v>194</v>
       </c>
     </row>
     <row r="75" spans="2:6" x14ac:dyDescent="0.25">
@@ -2321,6 +4227,7 @@
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
KeyAssigner: updating pin map
</commit_message>
<xml_diff>
--- a/PolysixKeyAssigner/KeyAssignerPinMap - Arduino Mega 2560.xlsx
+++ b/PolysixKeyAssigner/KeyAssignerPinMap - Arduino Mega 2560.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="197">
   <si>
     <t>Pin Number</t>
   </si>
@@ -604,6 +604,12 @@
   </si>
   <si>
     <t>Input (Pullup)</t>
+  </si>
+  <si>
+    <t>Serial3 to MIDI</t>
+  </si>
+  <si>
+    <t>Switch - Chord Mem</t>
   </si>
 </sst>
 </file>
@@ -2607,6 +2613,336 @@
     </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>515732</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>154781</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1064459" cy="436786"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="TextBox 11"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6909388" y="1952625"/>
+          <a:ext cx="1064459" cy="436786"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>Both</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t> Gnd Used</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>(Black Wires)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>309562</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>59531</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>654844</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="Straight Arrow Connector 13"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7727156" y="2393156"/>
+          <a:ext cx="345282" cy="797719"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>166687</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>59531</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>511969</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="58" name="Straight Arrow Connector 57"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7584281" y="2393156"/>
+          <a:ext cx="345282" cy="797719"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>558949</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>83344</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="978025" cy="436786"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="59" name="TextBox 58"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6952605" y="5464969"/>
+          <a:ext cx="978025" cy="436786"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>Both</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t> 5V Used</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>(Red Wires)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>464344</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>631031</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>35719</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="63" name="Straight Arrow Connector 62"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7881938" y="5191125"/>
+          <a:ext cx="166687" cy="226219"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>297656</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>119064</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>535782</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="64" name="Straight Arrow Connector 63"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7715250" y="5143502"/>
+          <a:ext cx="238126" cy="285748"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2899,8 +3235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:K105"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L77" sqref="K71:L77"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.28515625" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -3302,6 +3638,12 @@
       <c r="D35" s="2" t="s">
         <v>76</v>
       </c>
+      <c r="E35" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" s="2">
@@ -3347,6 +3689,12 @@
       <c r="D38" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="E38" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" s="2">
@@ -4217,7 +4565,7 @@
       </c>
       <c r="E105" s="6">
         <f>COUNTA(E4:E103)</f>
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
KeyAssigner: update pinmap again
</commit_message>
<xml_diff>
--- a/PolysixKeyAssigner/KeyAssignerPinMap - Arduino Mega 2560.xlsx
+++ b/PolysixKeyAssigner/KeyAssignerPinMap - Arduino Mega 2560.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="201">
   <si>
     <t>Pin Number</t>
   </si>
@@ -591,9 +591,6 @@
     <t>Serial3 from MIDI</t>
   </si>
   <si>
-    <t>Switch - Porta Pedal</t>
-  </si>
-  <si>
     <t>Num Pins</t>
   </si>
   <si>
@@ -609,7 +606,22 @@
     <t>Serial3 to MIDI</t>
   </si>
   <si>
-    <t>Switch - Chord Mem</t>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>Purple</t>
+  </si>
+  <si>
+    <t>Yellow</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Switch - Chord Mem (Porta)</t>
   </si>
 </sst>
 </file>
@@ -3235,8 +3247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:K105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.28515625" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -3489,10 +3501,13 @@
         <v>164</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>190</v>
+        <v>200</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
@@ -3511,6 +3526,9 @@
       <c r="F24" s="5" t="s">
         <v>158</v>
       </c>
+      <c r="G24" s="4" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" s="2">
@@ -3528,6 +3546,9 @@
       <c r="F25" s="5" t="s">
         <v>158</v>
       </c>
+      <c r="G25" s="4" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26" s="2">
@@ -3606,7 +3627,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="2">
         <v>25</v>
       </c>
@@ -3617,7 +3638,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:7" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B34" s="2">
         <v>26</v>
       </c>
@@ -3628,7 +3649,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="2">
         <v>64</v>
       </c>
@@ -3639,13 +3660,13 @@
         <v>76</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F35" s="5" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="2">
         <v>63</v>
       </c>
@@ -3662,7 +3683,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="2">
         <v>13</v>
       </c>
@@ -3679,7 +3700,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B38" s="2">
         <v>12</v>
       </c>
@@ -3689,14 +3710,8 @@
       <c r="D38" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E38" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B39" s="2">
         <v>46</v>
       </c>
@@ -3710,10 +3725,13 @@
         <v>183</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B40" s="2">
         <v>45</v>
       </c>
@@ -3729,8 +3747,11 @@
       <c r="F40" s="5" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G40" s="4" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B41" s="2">
         <v>44</v>
       </c>
@@ -3741,13 +3762,16 @@
         <v>47</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F41" s="5" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G41" s="4" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B42" s="2">
         <v>43</v>
       </c>
@@ -3758,13 +3782,16 @@
         <v>46</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F42" s="5" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G42" s="4" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B43" s="2">
         <v>78</v>
       </c>
@@ -3781,7 +3808,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B44" s="2">
         <v>77</v>
       </c>
@@ -3798,7 +3825,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B45" s="2">
         <v>76</v>
       </c>
@@ -3815,7 +3842,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B46" s="2">
         <v>75</v>
       </c>
@@ -3832,7 +3859,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B47" s="2">
         <v>74</v>
       </c>
@@ -3849,7 +3876,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B48" s="2">
         <v>73</v>
       </c>
@@ -4138,7 +4165,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B65" s="2">
         <v>40</v>
       </c>
@@ -4155,7 +4182,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B66" s="2">
         <v>39</v>
       </c>
@@ -4172,7 +4199,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B67" s="2">
         <v>38</v>
       </c>
@@ -4189,7 +4216,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B68" s="2">
         <v>37</v>
       </c>
@@ -4200,7 +4227,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B69" s="2">
         <v>36</v>
       </c>
@@ -4211,7 +4238,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B70" s="2">
         <v>35</v>
       </c>
@@ -4222,7 +4249,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B71" s="2">
         <v>22</v>
       </c>
@@ -4233,7 +4260,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B72" s="2">
         <v>21</v>
       </c>
@@ -4244,7 +4271,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B73" s="2">
         <v>20</v>
       </c>
@@ -4255,7 +4282,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="74" spans="2:6" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:7" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B74" s="2">
         <v>19</v>
       </c>
@@ -4269,10 +4296,13 @@
         <v>188</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+      <c r="G74" s="4" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B75" s="2">
         <v>11</v>
       </c>
@@ -4283,7 +4313,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B76" s="2">
         <v>32</v>
       </c>
@@ -4294,7 +4324,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B77" s="2">
         <v>62</v>
       </c>
@@ -4305,7 +4335,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B78" s="2">
         <v>81</v>
       </c>
@@ -4316,7 +4346,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B79" s="2">
         <v>99</v>
       </c>
@@ -4327,7 +4357,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B80" s="2">
         <v>30</v>
       </c>
@@ -4561,11 +4591,11 @@
     </row>
     <row r="105" spans="2:5" ht="15" x14ac:dyDescent="0.25">
       <c r="D105" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E105" s="6">
         <f>COUNTA(E4:E103)</f>
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
KeyAssigner: Arp seq is now 16 steps
</commit_message>
<xml_diff>
--- a/PolysixKeyAssigner/KeyAssignerPinMap - Arduino Mega 2560.xlsx
+++ b/PolysixKeyAssigner/KeyAssignerPinMap - Arduino Mega 2560.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="17235" windowHeight="9270"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="17235" windowHeight="9210"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="202">
   <si>
     <t>Pin Number</t>
   </si>
@@ -622,6 +622,9 @@
   </si>
   <si>
     <t>Switch - Chord Mem (Porta)</t>
+  </si>
+  <si>
+    <t>AudioIn (Analog Comparator)</t>
   </si>
 </sst>
 </file>
@@ -720,13 +723,13 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFCC00CC"/>
       <color rgb="FF00FF00"/>
       <color rgb="FF008000"/>
       <color rgb="FF00CC00"/>
       <color rgb="FF0000FF"/>
       <color rgb="FF00FFFF"/>
       <color rgb="FFFF00FF"/>
-      <color rgb="FFCC00CC"/>
     </mruColors>
   </colors>
   <extLst>
@@ -741,524 +744,1397 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>326517</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>11903</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>861014</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>35718</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>22801</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>19843</xdr:rowOff>
+      <xdr:colOff>368083</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>43880</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="62" name="Group 61"/>
+        <xdr:cNvPr id="13" name="Group 12"/>
         <xdr:cNvGrpSpPr/>
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="7744111" y="2881309"/>
-          <a:ext cx="4923128" cy="2341565"/>
-          <a:chOff x="8006049" y="10548935"/>
-          <a:chExt cx="4875503" cy="2341565"/>
+          <a:off x="7447918" y="2057949"/>
+          <a:ext cx="5976742" cy="4045296"/>
+          <a:chOff x="7111795" y="1952625"/>
+          <a:chExt cx="5757850" cy="3949130"/>
         </a:xfrm>
       </xdr:grpSpPr>
-      <xdr:pic>
-        <xdr:nvPicPr>
-          <xdr:cNvPr id="2" name="Picture 1" descr="http://flipmu.com/files/2011/12/ArduinoMega2650Front_21.jpg"/>
-          <xdr:cNvPicPr>
-            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-          </xdr:cNvPicPr>
-        </xdr:nvPicPr>
-        <xdr:blipFill rotWithShape="1">
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-            <a:extLst>
-              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-              </a:ext>
-            </a:extLst>
-          </a:blip>
-          <a:srcRect t="5948" r="4153" b="9875"/>
-          <a:stretch/>
-        </xdr:blipFill>
-        <xdr:spPr bwMode="auto">
-          <a:xfrm rot="10800000">
-            <a:off x="8006049" y="10548935"/>
-            <a:ext cx="4875503" cy="2341565"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:extLst>
-            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-                <a:solidFill>
-                  <a:srgbClr val="FFFFFF"/>
-                </a:solidFill>
-              </a14:hiddenFill>
-            </a:ext>
-          </a:extLst>
-        </xdr:spPr>
-      </xdr:pic>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="3" name="Oval 2"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="9815802" y="12668249"/>
-            <a:ext cx="124476" cy="127722"/>
-          </a:xfrm>
-          <a:prstGeom prst="ellipse">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:srgbClr val="00FF00"/>
-          </a:solidFill>
-          <a:ln>
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="4" name="Oval 3"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="9911052" y="12668249"/>
-            <a:ext cx="124476" cy="127722"/>
-          </a:xfrm>
-          <a:prstGeom prst="ellipse">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:srgbClr val="00FF00"/>
-          </a:solidFill>
-          <a:ln>
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="5" name="Oval 4"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="10023620" y="12668249"/>
-            <a:ext cx="124476" cy="127722"/>
-          </a:xfrm>
-          <a:prstGeom prst="ellipse">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:srgbClr val="00FF00"/>
-          </a:solidFill>
-          <a:ln>
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="6" name="Oval 5"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="9261260" y="12668249"/>
-            <a:ext cx="124476" cy="127722"/>
-          </a:xfrm>
-          <a:prstGeom prst="ellipse">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:srgbClr val="FFFF00"/>
-          </a:solidFill>
-          <a:ln>
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="7" name="Oval 6"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="9140754" y="12668249"/>
-            <a:ext cx="124476" cy="127722"/>
-          </a:xfrm>
-          <a:prstGeom prst="ellipse">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:srgbClr val="FFFF00"/>
-          </a:solidFill>
-          <a:ln>
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="8" name="Oval 7"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="8924998" y="12668249"/>
-            <a:ext cx="124476" cy="127722"/>
-          </a:xfrm>
-          <a:prstGeom prst="ellipse">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:srgbClr val="00FF00"/>
-          </a:solidFill>
-          <a:ln>
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="9" name="Oval 8"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="8821088" y="12668249"/>
-            <a:ext cx="124476" cy="127722"/>
-          </a:xfrm>
-          <a:prstGeom prst="ellipse">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:srgbClr val="00FF00"/>
-          </a:solidFill>
-          <a:ln>
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="10" name="Oval 9"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="8708520" y="12668249"/>
-            <a:ext cx="124476" cy="127722"/>
-          </a:xfrm>
-          <a:prstGeom prst="ellipse">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:srgbClr val="0000FF"/>
-          </a:solidFill>
-          <a:ln>
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="11" name="Oval 10"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="8612549" y="12668249"/>
-            <a:ext cx="124476" cy="127722"/>
-          </a:xfrm>
-          <a:prstGeom prst="ellipse">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:srgbClr val="0000FF"/>
-          </a:solidFill>
-          <a:ln>
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent1"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
       <xdr:grpSp>
         <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="31" name="Group 30"/>
+          <xdr:cNvPr id="62" name="Group 61"/>
           <xdr:cNvGrpSpPr/>
         </xdr:nvGrpSpPr>
         <xdr:grpSpPr>
           <a:xfrm>
-            <a:off x="8162997" y="12256634"/>
-            <a:ext cx="215601" cy="421358"/>
-            <a:chOff x="8238970" y="9493250"/>
-            <a:chExt cx="215601" cy="427028"/>
+            <a:off x="7946517" y="2881309"/>
+            <a:ext cx="4923128" cy="2341565"/>
+            <a:chOff x="8006049" y="10548935"/>
+            <a:chExt cx="4875503" cy="2341565"/>
           </a:xfrm>
-          <a:solidFill>
-            <a:srgbClr val="FF0000"/>
-          </a:solidFill>
         </xdr:grpSpPr>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="2" name="Picture 1" descr="http://flipmu.com/files/2011/12/ArduinoMega2650Front_21.jpg"/>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill rotWithShape="1">
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+              <a:extLst>
+                <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                  <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+                </a:ext>
+              </a:extLst>
+            </a:blip>
+            <a:srcRect t="5948" r="4153" b="9875"/>
+            <a:stretch/>
+          </xdr:blipFill>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm rot="10800000">
+              <a:off x="8006049" y="10548935"/>
+              <a:ext cx="4875503" cy="2341565"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:pic>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3" name="Oval 2"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9815802" y="12668249"/>
+              <a:ext cx="124476" cy="127722"/>
+            </a:xfrm>
+            <a:prstGeom prst="ellipse">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="00FF00"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4" name="Oval 3"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9911052" y="12668249"/>
+              <a:ext cx="124476" cy="127722"/>
+            </a:xfrm>
+            <a:prstGeom prst="ellipse">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="00FF00"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="5" name="Oval 4"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="10023620" y="12668249"/>
+              <a:ext cx="124476" cy="127722"/>
+            </a:xfrm>
+            <a:prstGeom prst="ellipse">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="00FF00"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="6" name="Oval 5"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9261260" y="12668249"/>
+              <a:ext cx="124476" cy="127722"/>
+            </a:xfrm>
+            <a:prstGeom prst="ellipse">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFF00"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="7" name="Oval 6"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9140754" y="12668249"/>
+              <a:ext cx="124476" cy="127722"/>
+            </a:xfrm>
+            <a:prstGeom prst="ellipse">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFF00"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="8" name="Oval 7"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8924998" y="12668249"/>
+              <a:ext cx="124476" cy="127722"/>
+            </a:xfrm>
+            <a:prstGeom prst="ellipse">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="00FF00"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9" name="Oval 8"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8821088" y="12668249"/>
+              <a:ext cx="124476" cy="127722"/>
+            </a:xfrm>
+            <a:prstGeom prst="ellipse">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="00FF00"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10" name="Oval 9"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8708520" y="12668249"/>
+              <a:ext cx="124476" cy="127722"/>
+            </a:xfrm>
+            <a:prstGeom prst="ellipse">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="0000FF"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="11" name="Oval 10"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8612549" y="12668249"/>
+              <a:ext cx="124476" cy="127722"/>
+            </a:xfrm>
+            <a:prstGeom prst="ellipse">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="0000FF"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
         <xdr:grpSp>
           <xdr:nvGrpSpPr>
-            <xdr:cNvPr id="21" name="Group 20"/>
+            <xdr:cNvPr id="31" name="Group 30"/>
             <xdr:cNvGrpSpPr/>
           </xdr:nvGrpSpPr>
           <xdr:grpSpPr>
             <a:xfrm>
-              <a:off x="8238970" y="9493250"/>
-              <a:ext cx="215601" cy="109527"/>
+              <a:off x="8162997" y="12256634"/>
+              <a:ext cx="215601" cy="421358"/>
+              <a:chOff x="8238970" y="9493250"/>
+              <a:chExt cx="215601" cy="427028"/>
+            </a:xfrm>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </xdr:grpSpPr>
+          <xdr:grpSp>
+            <xdr:nvGrpSpPr>
+              <xdr:cNvPr id="21" name="Group 20"/>
+              <xdr:cNvGrpSpPr/>
+            </xdr:nvGrpSpPr>
+            <xdr:grpSpPr>
+              <a:xfrm>
+                <a:off x="8238970" y="9493250"/>
+                <a:ext cx="215601" cy="109527"/>
+                <a:chOff x="8238970" y="9493250"/>
+                <a:chExt cx="215601" cy="109527"/>
+              </a:xfrm>
+              <a:grpFill/>
+            </xdr:grpSpPr>
+            <xdr:sp macro="" textlink="">
+              <xdr:nvSpPr>
+                <xdr:cNvPr id="19" name="Oval 18"/>
+                <xdr:cNvSpPr/>
+              </xdr:nvSpPr>
+              <xdr:spPr>
+                <a:xfrm>
+                  <a:off x="8238970" y="9493250"/>
+                  <a:ext cx="111280" cy="109527"/>
+                </a:xfrm>
+                <a:prstGeom prst="ellipse">
+                  <a:avLst/>
+                </a:prstGeom>
+                <a:grpFill/>
+                <a:ln>
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                </a:ln>
+              </xdr:spPr>
+              <xdr:style>
+                <a:lnRef idx="2">
+                  <a:schemeClr val="accent1">
+                    <a:shade val="50000"/>
+                  </a:schemeClr>
+                </a:lnRef>
+                <a:fillRef idx="1">
+                  <a:schemeClr val="accent1"/>
+                </a:fillRef>
+                <a:effectRef idx="0">
+                  <a:schemeClr val="accent1"/>
+                </a:effectRef>
+                <a:fontRef idx="minor">
+                  <a:schemeClr val="lt1"/>
+                </a:fontRef>
+              </xdr:style>
+              <xdr:txBody>
+                <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr algn="l"/>
+                  <a:endParaRPr lang="en-US" sz="1100"/>
+                </a:p>
+              </xdr:txBody>
+            </xdr:sp>
+            <xdr:sp macro="" textlink="">
+              <xdr:nvSpPr>
+                <xdr:cNvPr id="20" name="Oval 19"/>
+                <xdr:cNvSpPr/>
+              </xdr:nvSpPr>
+              <xdr:spPr>
+                <a:xfrm>
+                  <a:off x="8343291" y="9493250"/>
+                  <a:ext cx="111280" cy="109527"/>
+                </a:xfrm>
+                <a:prstGeom prst="ellipse">
+                  <a:avLst/>
+                </a:prstGeom>
+                <a:grpFill/>
+                <a:ln>
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                </a:ln>
+              </xdr:spPr>
+              <xdr:style>
+                <a:lnRef idx="2">
+                  <a:schemeClr val="accent1">
+                    <a:shade val="50000"/>
+                  </a:schemeClr>
+                </a:lnRef>
+                <a:fillRef idx="1">
+                  <a:schemeClr val="accent1"/>
+                </a:fillRef>
+                <a:effectRef idx="0">
+                  <a:schemeClr val="accent1"/>
+                </a:effectRef>
+                <a:fontRef idx="minor">
+                  <a:schemeClr val="lt1"/>
+                </a:fontRef>
+              </xdr:style>
+              <xdr:txBody>
+                <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr algn="l"/>
+                  <a:endParaRPr lang="en-US" sz="1100"/>
+                </a:p>
+              </xdr:txBody>
+            </xdr:sp>
+          </xdr:grpSp>
+          <xdr:grpSp>
+            <xdr:nvGrpSpPr>
+              <xdr:cNvPr id="22" name="Group 21"/>
+              <xdr:cNvGrpSpPr/>
+            </xdr:nvGrpSpPr>
+            <xdr:grpSpPr>
+              <a:xfrm>
+                <a:off x="8238970" y="9599084"/>
+                <a:ext cx="215601" cy="109527"/>
+                <a:chOff x="8238970" y="9493250"/>
+                <a:chExt cx="215601" cy="109527"/>
+              </a:xfrm>
+              <a:grpFill/>
+            </xdr:grpSpPr>
+            <xdr:sp macro="" textlink="">
+              <xdr:nvSpPr>
+                <xdr:cNvPr id="23" name="Oval 22"/>
+                <xdr:cNvSpPr/>
+              </xdr:nvSpPr>
+              <xdr:spPr>
+                <a:xfrm>
+                  <a:off x="8238970" y="9493250"/>
+                  <a:ext cx="111280" cy="109527"/>
+                </a:xfrm>
+                <a:prstGeom prst="ellipse">
+                  <a:avLst/>
+                </a:prstGeom>
+                <a:grpFill/>
+                <a:ln>
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                </a:ln>
+              </xdr:spPr>
+              <xdr:style>
+                <a:lnRef idx="2">
+                  <a:schemeClr val="accent1">
+                    <a:shade val="50000"/>
+                  </a:schemeClr>
+                </a:lnRef>
+                <a:fillRef idx="1">
+                  <a:schemeClr val="accent1"/>
+                </a:fillRef>
+                <a:effectRef idx="0">
+                  <a:schemeClr val="accent1"/>
+                </a:effectRef>
+                <a:fontRef idx="minor">
+                  <a:schemeClr val="lt1"/>
+                </a:fontRef>
+              </xdr:style>
+              <xdr:txBody>
+                <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr algn="l"/>
+                  <a:endParaRPr lang="en-US" sz="1100"/>
+                </a:p>
+              </xdr:txBody>
+            </xdr:sp>
+            <xdr:sp macro="" textlink="">
+              <xdr:nvSpPr>
+                <xdr:cNvPr id="24" name="Oval 23"/>
+                <xdr:cNvSpPr/>
+              </xdr:nvSpPr>
+              <xdr:spPr>
+                <a:xfrm>
+                  <a:off x="8343291" y="9493250"/>
+                  <a:ext cx="111280" cy="109527"/>
+                </a:xfrm>
+                <a:prstGeom prst="ellipse">
+                  <a:avLst/>
+                </a:prstGeom>
+                <a:grpFill/>
+                <a:ln>
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                </a:ln>
+              </xdr:spPr>
+              <xdr:style>
+                <a:lnRef idx="2">
+                  <a:schemeClr val="accent1">
+                    <a:shade val="50000"/>
+                  </a:schemeClr>
+                </a:lnRef>
+                <a:fillRef idx="1">
+                  <a:schemeClr val="accent1"/>
+                </a:fillRef>
+                <a:effectRef idx="0">
+                  <a:schemeClr val="accent1"/>
+                </a:effectRef>
+                <a:fontRef idx="minor">
+                  <a:schemeClr val="lt1"/>
+                </a:fontRef>
+              </xdr:style>
+              <xdr:txBody>
+                <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr algn="l"/>
+                  <a:endParaRPr lang="en-US" sz="1100"/>
+                </a:p>
+              </xdr:txBody>
+            </xdr:sp>
+          </xdr:grpSp>
+          <xdr:grpSp>
+            <xdr:nvGrpSpPr>
+              <xdr:cNvPr id="25" name="Group 24"/>
+              <xdr:cNvGrpSpPr/>
+            </xdr:nvGrpSpPr>
+            <xdr:grpSpPr>
+              <a:xfrm>
+                <a:off x="8238970" y="9704918"/>
+                <a:ext cx="215601" cy="109527"/>
+                <a:chOff x="8238970" y="9493250"/>
+                <a:chExt cx="215601" cy="109527"/>
+              </a:xfrm>
+              <a:grpFill/>
+            </xdr:grpSpPr>
+            <xdr:sp macro="" textlink="">
+              <xdr:nvSpPr>
+                <xdr:cNvPr id="26" name="Oval 25"/>
+                <xdr:cNvSpPr/>
+              </xdr:nvSpPr>
+              <xdr:spPr>
+                <a:xfrm>
+                  <a:off x="8238970" y="9493250"/>
+                  <a:ext cx="111280" cy="109527"/>
+                </a:xfrm>
+                <a:prstGeom prst="ellipse">
+                  <a:avLst/>
+                </a:prstGeom>
+                <a:grpFill/>
+                <a:ln>
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                </a:ln>
+              </xdr:spPr>
+              <xdr:style>
+                <a:lnRef idx="2">
+                  <a:schemeClr val="accent1">
+                    <a:shade val="50000"/>
+                  </a:schemeClr>
+                </a:lnRef>
+                <a:fillRef idx="1">
+                  <a:schemeClr val="accent1"/>
+                </a:fillRef>
+                <a:effectRef idx="0">
+                  <a:schemeClr val="accent1"/>
+                </a:effectRef>
+                <a:fontRef idx="minor">
+                  <a:schemeClr val="lt1"/>
+                </a:fontRef>
+              </xdr:style>
+              <xdr:txBody>
+                <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr algn="l"/>
+                  <a:endParaRPr lang="en-US" sz="1100"/>
+                </a:p>
+              </xdr:txBody>
+            </xdr:sp>
+            <xdr:sp macro="" textlink="">
+              <xdr:nvSpPr>
+                <xdr:cNvPr id="27" name="Oval 26"/>
+                <xdr:cNvSpPr/>
+              </xdr:nvSpPr>
+              <xdr:spPr>
+                <a:xfrm>
+                  <a:off x="8343291" y="9493250"/>
+                  <a:ext cx="111280" cy="109527"/>
+                </a:xfrm>
+                <a:prstGeom prst="ellipse">
+                  <a:avLst/>
+                </a:prstGeom>
+                <a:grpFill/>
+                <a:ln>
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                </a:ln>
+              </xdr:spPr>
+              <xdr:style>
+                <a:lnRef idx="2">
+                  <a:schemeClr val="accent1">
+                    <a:shade val="50000"/>
+                  </a:schemeClr>
+                </a:lnRef>
+                <a:fillRef idx="1">
+                  <a:schemeClr val="accent1"/>
+                </a:fillRef>
+                <a:effectRef idx="0">
+                  <a:schemeClr val="accent1"/>
+                </a:effectRef>
+                <a:fontRef idx="minor">
+                  <a:schemeClr val="lt1"/>
+                </a:fontRef>
+              </xdr:style>
+              <xdr:txBody>
+                <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr algn="l"/>
+                  <a:endParaRPr lang="en-US" sz="1100"/>
+                </a:p>
+              </xdr:txBody>
+            </xdr:sp>
+          </xdr:grpSp>
+          <xdr:grpSp>
+            <xdr:nvGrpSpPr>
+              <xdr:cNvPr id="28" name="Group 27"/>
+              <xdr:cNvGrpSpPr/>
+            </xdr:nvGrpSpPr>
+            <xdr:grpSpPr>
+              <a:xfrm>
+                <a:off x="8238970" y="9810751"/>
+                <a:ext cx="215601" cy="109527"/>
+                <a:chOff x="8238970" y="9493250"/>
+                <a:chExt cx="215601" cy="109527"/>
+              </a:xfrm>
+              <a:grpFill/>
+            </xdr:grpSpPr>
+            <xdr:sp macro="" textlink="">
+              <xdr:nvSpPr>
+                <xdr:cNvPr id="29" name="Oval 28"/>
+                <xdr:cNvSpPr/>
+              </xdr:nvSpPr>
+              <xdr:spPr>
+                <a:xfrm>
+                  <a:off x="8238970" y="9493250"/>
+                  <a:ext cx="111280" cy="109527"/>
+                </a:xfrm>
+                <a:prstGeom prst="ellipse">
+                  <a:avLst/>
+                </a:prstGeom>
+                <a:grpFill/>
+                <a:ln>
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                </a:ln>
+              </xdr:spPr>
+              <xdr:style>
+                <a:lnRef idx="2">
+                  <a:schemeClr val="accent1">
+                    <a:shade val="50000"/>
+                  </a:schemeClr>
+                </a:lnRef>
+                <a:fillRef idx="1">
+                  <a:schemeClr val="accent1"/>
+                </a:fillRef>
+                <a:effectRef idx="0">
+                  <a:schemeClr val="accent1"/>
+                </a:effectRef>
+                <a:fontRef idx="minor">
+                  <a:schemeClr val="lt1"/>
+                </a:fontRef>
+              </xdr:style>
+              <xdr:txBody>
+                <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr algn="l"/>
+                  <a:endParaRPr lang="en-US" sz="1100"/>
+                </a:p>
+              </xdr:txBody>
+            </xdr:sp>
+            <xdr:sp macro="" textlink="">
+              <xdr:nvSpPr>
+                <xdr:cNvPr id="30" name="Oval 29"/>
+                <xdr:cNvSpPr/>
+              </xdr:nvSpPr>
+              <xdr:spPr>
+                <a:xfrm>
+                  <a:off x="8343291" y="9493250"/>
+                  <a:ext cx="111280" cy="109527"/>
+                </a:xfrm>
+                <a:prstGeom prst="ellipse">
+                  <a:avLst/>
+                </a:prstGeom>
+                <a:grpFill/>
+                <a:ln>
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                </a:ln>
+              </xdr:spPr>
+              <xdr:style>
+                <a:lnRef idx="2">
+                  <a:schemeClr val="accent1">
+                    <a:shade val="50000"/>
+                  </a:schemeClr>
+                </a:lnRef>
+                <a:fillRef idx="1">
+                  <a:schemeClr val="accent1"/>
+                </a:fillRef>
+                <a:effectRef idx="0">
+                  <a:schemeClr val="accent1"/>
+                </a:effectRef>
+                <a:fontRef idx="minor">
+                  <a:schemeClr val="lt1"/>
+                </a:fontRef>
+              </xdr:style>
+              <xdr:txBody>
+                <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr algn="l"/>
+                  <a:endParaRPr lang="en-US" sz="1100"/>
+                </a:p>
+              </xdr:txBody>
+            </xdr:sp>
+          </xdr:grpSp>
+        </xdr:grpSp>
+        <xdr:grpSp>
+          <xdr:nvGrpSpPr>
+            <xdr:cNvPr id="32" name="Group 31"/>
+            <xdr:cNvGrpSpPr/>
+          </xdr:nvGrpSpPr>
+          <xdr:grpSpPr>
+            <a:xfrm>
+              <a:off x="8162997" y="11825741"/>
+              <a:ext cx="215601" cy="422492"/>
+              <a:chOff x="8238970" y="9493250"/>
+              <a:chExt cx="215601" cy="427028"/>
+            </a:xfrm>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </xdr:grpSpPr>
+          <xdr:grpSp>
+            <xdr:nvGrpSpPr>
+              <xdr:cNvPr id="33" name="Group 32"/>
+              <xdr:cNvGrpSpPr/>
+            </xdr:nvGrpSpPr>
+            <xdr:grpSpPr>
+              <a:xfrm>
+                <a:off x="8238970" y="9493250"/>
+                <a:ext cx="215601" cy="109527"/>
+                <a:chOff x="8238970" y="9493250"/>
+                <a:chExt cx="215601" cy="109527"/>
+              </a:xfrm>
+              <a:grpFill/>
+            </xdr:grpSpPr>
+            <xdr:sp macro="" textlink="">
+              <xdr:nvSpPr>
+                <xdr:cNvPr id="43" name="Oval 42"/>
+                <xdr:cNvSpPr/>
+              </xdr:nvSpPr>
+              <xdr:spPr>
+                <a:xfrm>
+                  <a:off x="8238970" y="9493250"/>
+                  <a:ext cx="111280" cy="109527"/>
+                </a:xfrm>
+                <a:prstGeom prst="ellipse">
+                  <a:avLst/>
+                </a:prstGeom>
+                <a:grpFill/>
+                <a:ln>
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                </a:ln>
+              </xdr:spPr>
+              <xdr:style>
+                <a:lnRef idx="2">
+                  <a:schemeClr val="accent1">
+                    <a:shade val="50000"/>
+                  </a:schemeClr>
+                </a:lnRef>
+                <a:fillRef idx="1">
+                  <a:schemeClr val="accent1"/>
+                </a:fillRef>
+                <a:effectRef idx="0">
+                  <a:schemeClr val="accent1"/>
+                </a:effectRef>
+                <a:fontRef idx="minor">
+                  <a:schemeClr val="lt1"/>
+                </a:fontRef>
+              </xdr:style>
+              <xdr:txBody>
+                <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr algn="l"/>
+                  <a:endParaRPr lang="en-US" sz="1100"/>
+                </a:p>
+              </xdr:txBody>
+            </xdr:sp>
+            <xdr:sp macro="" textlink="">
+              <xdr:nvSpPr>
+                <xdr:cNvPr id="44" name="Oval 43"/>
+                <xdr:cNvSpPr/>
+              </xdr:nvSpPr>
+              <xdr:spPr>
+                <a:xfrm>
+                  <a:off x="8343291" y="9493250"/>
+                  <a:ext cx="111280" cy="109527"/>
+                </a:xfrm>
+                <a:prstGeom prst="ellipse">
+                  <a:avLst/>
+                </a:prstGeom>
+                <a:grpFill/>
+                <a:ln>
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                </a:ln>
+              </xdr:spPr>
+              <xdr:style>
+                <a:lnRef idx="2">
+                  <a:schemeClr val="accent1">
+                    <a:shade val="50000"/>
+                  </a:schemeClr>
+                </a:lnRef>
+                <a:fillRef idx="1">
+                  <a:schemeClr val="accent1"/>
+                </a:fillRef>
+                <a:effectRef idx="0">
+                  <a:schemeClr val="accent1"/>
+                </a:effectRef>
+                <a:fontRef idx="minor">
+                  <a:schemeClr val="lt1"/>
+                </a:fontRef>
+              </xdr:style>
+              <xdr:txBody>
+                <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr algn="l"/>
+                  <a:endParaRPr lang="en-US" sz="1100"/>
+                </a:p>
+              </xdr:txBody>
+            </xdr:sp>
+          </xdr:grpSp>
+          <xdr:grpSp>
+            <xdr:nvGrpSpPr>
+              <xdr:cNvPr id="34" name="Group 33"/>
+              <xdr:cNvGrpSpPr/>
+            </xdr:nvGrpSpPr>
+            <xdr:grpSpPr>
+              <a:xfrm>
+                <a:off x="8238970" y="9599084"/>
+                <a:ext cx="215601" cy="109527"/>
+                <a:chOff x="8238970" y="9493250"/>
+                <a:chExt cx="215601" cy="109527"/>
+              </a:xfrm>
+              <a:grpFill/>
+            </xdr:grpSpPr>
+            <xdr:sp macro="" textlink="">
+              <xdr:nvSpPr>
+                <xdr:cNvPr id="41" name="Oval 40"/>
+                <xdr:cNvSpPr/>
+              </xdr:nvSpPr>
+              <xdr:spPr>
+                <a:xfrm>
+                  <a:off x="8238970" y="9493250"/>
+                  <a:ext cx="111280" cy="109527"/>
+                </a:xfrm>
+                <a:prstGeom prst="ellipse">
+                  <a:avLst/>
+                </a:prstGeom>
+                <a:grpFill/>
+                <a:ln>
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                </a:ln>
+              </xdr:spPr>
+              <xdr:style>
+                <a:lnRef idx="2">
+                  <a:schemeClr val="accent1">
+                    <a:shade val="50000"/>
+                  </a:schemeClr>
+                </a:lnRef>
+                <a:fillRef idx="1">
+                  <a:schemeClr val="accent1"/>
+                </a:fillRef>
+                <a:effectRef idx="0">
+                  <a:schemeClr val="accent1"/>
+                </a:effectRef>
+                <a:fontRef idx="minor">
+                  <a:schemeClr val="lt1"/>
+                </a:fontRef>
+              </xdr:style>
+              <xdr:txBody>
+                <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr algn="l"/>
+                  <a:endParaRPr lang="en-US" sz="1100"/>
+                </a:p>
+              </xdr:txBody>
+            </xdr:sp>
+            <xdr:sp macro="" textlink="">
+              <xdr:nvSpPr>
+                <xdr:cNvPr id="42" name="Oval 41"/>
+                <xdr:cNvSpPr/>
+              </xdr:nvSpPr>
+              <xdr:spPr>
+                <a:xfrm>
+                  <a:off x="8343291" y="9493250"/>
+                  <a:ext cx="111280" cy="109527"/>
+                </a:xfrm>
+                <a:prstGeom prst="ellipse">
+                  <a:avLst/>
+                </a:prstGeom>
+                <a:grpFill/>
+                <a:ln>
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                </a:ln>
+              </xdr:spPr>
+              <xdr:style>
+                <a:lnRef idx="2">
+                  <a:schemeClr val="accent1">
+                    <a:shade val="50000"/>
+                  </a:schemeClr>
+                </a:lnRef>
+                <a:fillRef idx="1">
+                  <a:schemeClr val="accent1"/>
+                </a:fillRef>
+                <a:effectRef idx="0">
+                  <a:schemeClr val="accent1"/>
+                </a:effectRef>
+                <a:fontRef idx="minor">
+                  <a:schemeClr val="lt1"/>
+                </a:fontRef>
+              </xdr:style>
+              <xdr:txBody>
+                <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr algn="l"/>
+                  <a:endParaRPr lang="en-US" sz="1100"/>
+                </a:p>
+              </xdr:txBody>
+            </xdr:sp>
+          </xdr:grpSp>
+          <xdr:grpSp>
+            <xdr:nvGrpSpPr>
+              <xdr:cNvPr id="35" name="Group 34"/>
+              <xdr:cNvGrpSpPr/>
+            </xdr:nvGrpSpPr>
+            <xdr:grpSpPr>
+              <a:xfrm>
+                <a:off x="8238970" y="9704918"/>
+                <a:ext cx="215601" cy="109527"/>
+                <a:chOff x="8238970" y="9493250"/>
+                <a:chExt cx="215601" cy="109527"/>
+              </a:xfrm>
+              <a:grpFill/>
+            </xdr:grpSpPr>
+            <xdr:sp macro="" textlink="">
+              <xdr:nvSpPr>
+                <xdr:cNvPr id="39" name="Oval 38"/>
+                <xdr:cNvSpPr/>
+              </xdr:nvSpPr>
+              <xdr:spPr>
+                <a:xfrm>
+                  <a:off x="8238970" y="9493250"/>
+                  <a:ext cx="111280" cy="109527"/>
+                </a:xfrm>
+                <a:prstGeom prst="ellipse">
+                  <a:avLst/>
+                </a:prstGeom>
+                <a:grpFill/>
+                <a:ln>
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                </a:ln>
+              </xdr:spPr>
+              <xdr:style>
+                <a:lnRef idx="2">
+                  <a:schemeClr val="accent1">
+                    <a:shade val="50000"/>
+                  </a:schemeClr>
+                </a:lnRef>
+                <a:fillRef idx="1">
+                  <a:schemeClr val="accent1"/>
+                </a:fillRef>
+                <a:effectRef idx="0">
+                  <a:schemeClr val="accent1"/>
+                </a:effectRef>
+                <a:fontRef idx="minor">
+                  <a:schemeClr val="lt1"/>
+                </a:fontRef>
+              </xdr:style>
+              <xdr:txBody>
+                <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr algn="l"/>
+                  <a:endParaRPr lang="en-US" sz="1100"/>
+                </a:p>
+              </xdr:txBody>
+            </xdr:sp>
+            <xdr:sp macro="" textlink="">
+              <xdr:nvSpPr>
+                <xdr:cNvPr id="40" name="Oval 39"/>
+                <xdr:cNvSpPr/>
+              </xdr:nvSpPr>
+              <xdr:spPr>
+                <a:xfrm>
+                  <a:off x="8343291" y="9493250"/>
+                  <a:ext cx="111280" cy="109527"/>
+                </a:xfrm>
+                <a:prstGeom prst="ellipse">
+                  <a:avLst/>
+                </a:prstGeom>
+                <a:grpFill/>
+                <a:ln>
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                </a:ln>
+              </xdr:spPr>
+              <xdr:style>
+                <a:lnRef idx="2">
+                  <a:schemeClr val="accent1">
+                    <a:shade val="50000"/>
+                  </a:schemeClr>
+                </a:lnRef>
+                <a:fillRef idx="1">
+                  <a:schemeClr val="accent1"/>
+                </a:fillRef>
+                <a:effectRef idx="0">
+                  <a:schemeClr val="accent1"/>
+                </a:effectRef>
+                <a:fontRef idx="minor">
+                  <a:schemeClr val="lt1"/>
+                </a:fontRef>
+              </xdr:style>
+              <xdr:txBody>
+                <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr algn="l"/>
+                  <a:endParaRPr lang="en-US" sz="1100"/>
+                </a:p>
+              </xdr:txBody>
+            </xdr:sp>
+          </xdr:grpSp>
+          <xdr:grpSp>
+            <xdr:nvGrpSpPr>
+              <xdr:cNvPr id="36" name="Group 35"/>
+              <xdr:cNvGrpSpPr/>
+            </xdr:nvGrpSpPr>
+            <xdr:grpSpPr>
+              <a:xfrm>
+                <a:off x="8238970" y="9810751"/>
+                <a:ext cx="215601" cy="109527"/>
+                <a:chOff x="8238970" y="9493250"/>
+                <a:chExt cx="215601" cy="109527"/>
+              </a:xfrm>
+              <a:grpFill/>
+            </xdr:grpSpPr>
+            <xdr:sp macro="" textlink="">
+              <xdr:nvSpPr>
+                <xdr:cNvPr id="37" name="Oval 36"/>
+                <xdr:cNvSpPr/>
+              </xdr:nvSpPr>
+              <xdr:spPr>
+                <a:xfrm>
+                  <a:off x="8238970" y="9493250"/>
+                  <a:ext cx="111280" cy="109527"/>
+                </a:xfrm>
+                <a:prstGeom prst="ellipse">
+                  <a:avLst/>
+                </a:prstGeom>
+                <a:grpFill/>
+                <a:ln>
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                </a:ln>
+              </xdr:spPr>
+              <xdr:style>
+                <a:lnRef idx="2">
+                  <a:schemeClr val="accent1">
+                    <a:shade val="50000"/>
+                  </a:schemeClr>
+                </a:lnRef>
+                <a:fillRef idx="1">
+                  <a:schemeClr val="accent1"/>
+                </a:fillRef>
+                <a:effectRef idx="0">
+                  <a:schemeClr val="accent1"/>
+                </a:effectRef>
+                <a:fontRef idx="minor">
+                  <a:schemeClr val="lt1"/>
+                </a:fontRef>
+              </xdr:style>
+              <xdr:txBody>
+                <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr algn="l"/>
+                  <a:endParaRPr lang="en-US" sz="1100"/>
+                </a:p>
+              </xdr:txBody>
+            </xdr:sp>
+            <xdr:sp macro="" textlink="">
+              <xdr:nvSpPr>
+                <xdr:cNvPr id="38" name="Oval 37"/>
+                <xdr:cNvSpPr/>
+              </xdr:nvSpPr>
+              <xdr:spPr>
+                <a:xfrm>
+                  <a:off x="8343291" y="9493250"/>
+                  <a:ext cx="111280" cy="109527"/>
+                </a:xfrm>
+                <a:prstGeom prst="ellipse">
+                  <a:avLst/>
+                </a:prstGeom>
+                <a:grpFill/>
+                <a:ln>
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                </a:ln>
+              </xdr:spPr>
+              <xdr:style>
+                <a:lnRef idx="2">
+                  <a:schemeClr val="accent1">
+                    <a:shade val="50000"/>
+                  </a:schemeClr>
+                </a:lnRef>
+                <a:fillRef idx="1">
+                  <a:schemeClr val="accent1"/>
+                </a:fillRef>
+                <a:effectRef idx="0">
+                  <a:schemeClr val="accent1"/>
+                </a:effectRef>
+                <a:fontRef idx="minor">
+                  <a:schemeClr val="lt1"/>
+                </a:fontRef>
+              </xdr:style>
+              <xdr:txBody>
+                <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr algn="l"/>
+                  <a:endParaRPr lang="en-US" sz="1100"/>
+                </a:p>
+              </xdr:txBody>
+            </xdr:sp>
+          </xdr:grpSp>
+        </xdr:grpSp>
+        <xdr:grpSp>
+          <xdr:nvGrpSpPr>
+            <xdr:cNvPr id="46" name="Group 45"/>
+            <xdr:cNvGrpSpPr/>
+          </xdr:nvGrpSpPr>
+          <xdr:grpSpPr>
+            <a:xfrm>
+              <a:off x="8162997" y="11393146"/>
+              <a:ext cx="215601" cy="106431"/>
               <a:chOff x="8238970" y="9493250"/>
               <a:chExt cx="215601" cy="109527"/>
             </a:xfrm>
-            <a:grpFill/>
+            <a:solidFill>
+              <a:srgbClr val="00FF00"/>
+            </a:solidFill>
           </xdr:grpSpPr>
           <xdr:sp macro="" textlink="">
             <xdr:nvSpPr>
-              <xdr:cNvPr id="19" name="Oval 18"/>
+              <xdr:cNvPr id="56" name="Oval 55"/>
               <xdr:cNvSpPr/>
             </xdr:nvSpPr>
             <xdr:spPr>
@@ -1303,7 +2179,7 @@
           </xdr:sp>
           <xdr:sp macro="" textlink="">
             <xdr:nvSpPr>
-              <xdr:cNvPr id="20" name="Oval 19"/>
+              <xdr:cNvPr id="57" name="Oval 56"/>
               <xdr:cNvSpPr/>
             </xdr:nvSpPr>
             <xdr:spPr>
@@ -1349,21 +2225,23 @@
         </xdr:grpSp>
         <xdr:grpSp>
           <xdr:nvGrpSpPr>
-            <xdr:cNvPr id="22" name="Group 21"/>
+            <xdr:cNvPr id="47" name="Group 46"/>
             <xdr:cNvGrpSpPr/>
           </xdr:nvGrpSpPr>
           <xdr:grpSpPr>
             <a:xfrm>
-              <a:off x="8238970" y="9599084"/>
-              <a:ext cx="215601" cy="109527"/>
+              <a:off x="8162997" y="11495855"/>
+              <a:ext cx="215601" cy="110399"/>
               <a:chOff x="8238970" y="9493250"/>
               <a:chExt cx="215601" cy="109527"/>
             </a:xfrm>
-            <a:grpFill/>
+            <a:solidFill>
+              <a:srgbClr val="00FF00"/>
+            </a:solidFill>
           </xdr:grpSpPr>
           <xdr:sp macro="" textlink="">
             <xdr:nvSpPr>
-              <xdr:cNvPr id="23" name="Oval 22"/>
+              <xdr:cNvPr id="54" name="Oval 53"/>
               <xdr:cNvSpPr/>
             </xdr:nvSpPr>
             <xdr:spPr>
@@ -1408,7 +2286,7 @@
           </xdr:sp>
           <xdr:sp macro="" textlink="">
             <xdr:nvSpPr>
-              <xdr:cNvPr id="24" name="Oval 23"/>
+              <xdr:cNvPr id="55" name="Oval 54"/>
               <xdr:cNvSpPr/>
             </xdr:nvSpPr>
             <xdr:spPr>
@@ -1454,21 +2332,23 @@
         </xdr:grpSp>
         <xdr:grpSp>
           <xdr:nvGrpSpPr>
-            <xdr:cNvPr id="25" name="Group 24"/>
+            <xdr:cNvPr id="48" name="Group 47"/>
             <xdr:cNvGrpSpPr/>
           </xdr:nvGrpSpPr>
           <xdr:grpSpPr>
             <a:xfrm>
-              <a:off x="8238970" y="9704918"/>
-              <a:ext cx="215601" cy="109527"/>
+              <a:off x="8162997" y="11602532"/>
+              <a:ext cx="215601" cy="106429"/>
               <a:chOff x="8238970" y="9493250"/>
               <a:chExt cx="215601" cy="109527"/>
             </a:xfrm>
-            <a:grpFill/>
+            <a:solidFill>
+              <a:srgbClr val="00FF00"/>
+            </a:solidFill>
           </xdr:grpSpPr>
           <xdr:sp macro="" textlink="">
             <xdr:nvSpPr>
-              <xdr:cNvPr id="26" name="Oval 25"/>
+              <xdr:cNvPr id="52" name="Oval 51"/>
               <xdr:cNvSpPr/>
             </xdr:nvSpPr>
             <xdr:spPr>
@@ -1513,7 +2393,7 @@
           </xdr:sp>
           <xdr:sp macro="" textlink="">
             <xdr:nvSpPr>
-              <xdr:cNvPr id="27" name="Oval 26"/>
+              <xdr:cNvPr id="53" name="Oval 52"/>
               <xdr:cNvSpPr/>
             </xdr:nvSpPr>
             <xdr:spPr>
@@ -1559,21 +2439,23 @@
         </xdr:grpSp>
         <xdr:grpSp>
           <xdr:nvGrpSpPr>
-            <xdr:cNvPr id="28" name="Group 27"/>
+            <xdr:cNvPr id="49" name="Group 48"/>
             <xdr:cNvGrpSpPr/>
           </xdr:nvGrpSpPr>
           <xdr:grpSpPr>
             <a:xfrm>
-              <a:off x="8238970" y="9810751"/>
-              <a:ext cx="215601" cy="109527"/>
+              <a:off x="8162997" y="11705238"/>
+              <a:ext cx="215601" cy="106431"/>
               <a:chOff x="8238970" y="9493250"/>
               <a:chExt cx="215601" cy="109527"/>
             </a:xfrm>
-            <a:grpFill/>
+            <a:solidFill>
+              <a:srgbClr val="00FF00"/>
+            </a:solidFill>
           </xdr:grpSpPr>
           <xdr:sp macro="" textlink="">
             <xdr:nvSpPr>
-              <xdr:cNvPr id="29" name="Oval 28"/>
+              <xdr:cNvPr id="50" name="Oval 49"/>
               <xdr:cNvSpPr/>
             </xdr:nvSpPr>
             <xdr:spPr>
@@ -1618,7 +2500,7 @@
           </xdr:sp>
           <xdr:sp macro="" textlink="">
             <xdr:nvSpPr>
-              <xdr:cNvPr id="30" name="Oval 29"/>
+              <xdr:cNvPr id="51" name="Oval 50"/>
               <xdr:cNvSpPr/>
             </xdr:nvSpPr>
             <xdr:spPr>
@@ -1662,474 +2544,22 @@
             </xdr:txBody>
           </xdr:sp>
         </xdr:grpSp>
-      </xdr:grpSp>
-      <xdr:grpSp>
-        <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="32" name="Group 31"/>
-          <xdr:cNvGrpSpPr/>
-        </xdr:nvGrpSpPr>
-        <xdr:grpSpPr>
-          <a:xfrm>
-            <a:off x="8162997" y="11825741"/>
-            <a:ext cx="215601" cy="422492"/>
-            <a:chOff x="8238970" y="9493250"/>
-            <a:chExt cx="215601" cy="427028"/>
-          </a:xfrm>
-          <a:solidFill>
-            <a:srgbClr val="FF0000"/>
-          </a:solidFill>
-        </xdr:grpSpPr>
-        <xdr:grpSp>
-          <xdr:nvGrpSpPr>
-            <xdr:cNvPr id="33" name="Group 32"/>
-            <xdr:cNvGrpSpPr/>
-          </xdr:nvGrpSpPr>
-          <xdr:grpSpPr>
-            <a:xfrm>
-              <a:off x="8238970" y="9493250"/>
-              <a:ext cx="215601" cy="109527"/>
-              <a:chOff x="8238970" y="9493250"/>
-              <a:chExt cx="215601" cy="109527"/>
-            </a:xfrm>
-            <a:grpFill/>
-          </xdr:grpSpPr>
-          <xdr:sp macro="" textlink="">
-            <xdr:nvSpPr>
-              <xdr:cNvPr id="43" name="Oval 42"/>
-              <xdr:cNvSpPr/>
-            </xdr:nvSpPr>
-            <xdr:spPr>
-              <a:xfrm>
-                <a:off x="8238970" y="9493250"/>
-                <a:ext cx="111280" cy="109527"/>
-              </a:xfrm>
-              <a:prstGeom prst="ellipse">
-                <a:avLst/>
-              </a:prstGeom>
-              <a:grpFill/>
-              <a:ln>
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-              </a:ln>
-            </xdr:spPr>
-            <xdr:style>
-              <a:lnRef idx="2">
-                <a:schemeClr val="accent1">
-                  <a:shade val="50000"/>
-                </a:schemeClr>
-              </a:lnRef>
-              <a:fillRef idx="1">
-                <a:schemeClr val="accent1"/>
-              </a:fillRef>
-              <a:effectRef idx="0">
-                <a:schemeClr val="accent1"/>
-              </a:effectRef>
-              <a:fontRef idx="minor">
-                <a:schemeClr val="lt1"/>
-              </a:fontRef>
-            </xdr:style>
-            <xdr:txBody>
-              <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr algn="l"/>
-                <a:endParaRPr lang="en-US" sz="1100"/>
-              </a:p>
-            </xdr:txBody>
-          </xdr:sp>
-          <xdr:sp macro="" textlink="">
-            <xdr:nvSpPr>
-              <xdr:cNvPr id="44" name="Oval 43"/>
-              <xdr:cNvSpPr/>
-            </xdr:nvSpPr>
-            <xdr:spPr>
-              <a:xfrm>
-                <a:off x="8343291" y="9493250"/>
-                <a:ext cx="111280" cy="109527"/>
-              </a:xfrm>
-              <a:prstGeom prst="ellipse">
-                <a:avLst/>
-              </a:prstGeom>
-              <a:grpFill/>
-              <a:ln>
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-              </a:ln>
-            </xdr:spPr>
-            <xdr:style>
-              <a:lnRef idx="2">
-                <a:schemeClr val="accent1">
-                  <a:shade val="50000"/>
-                </a:schemeClr>
-              </a:lnRef>
-              <a:fillRef idx="1">
-                <a:schemeClr val="accent1"/>
-              </a:fillRef>
-              <a:effectRef idx="0">
-                <a:schemeClr val="accent1"/>
-              </a:effectRef>
-              <a:fontRef idx="minor">
-                <a:schemeClr val="lt1"/>
-              </a:fontRef>
-            </xdr:style>
-            <xdr:txBody>
-              <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr algn="l"/>
-                <a:endParaRPr lang="en-US" sz="1100"/>
-              </a:p>
-            </xdr:txBody>
-          </xdr:sp>
-        </xdr:grpSp>
-        <xdr:grpSp>
-          <xdr:nvGrpSpPr>
-            <xdr:cNvPr id="34" name="Group 33"/>
-            <xdr:cNvGrpSpPr/>
-          </xdr:nvGrpSpPr>
-          <xdr:grpSpPr>
-            <a:xfrm>
-              <a:off x="8238970" y="9599084"/>
-              <a:ext cx="215601" cy="109527"/>
-              <a:chOff x="8238970" y="9493250"/>
-              <a:chExt cx="215601" cy="109527"/>
-            </a:xfrm>
-            <a:grpFill/>
-          </xdr:grpSpPr>
-          <xdr:sp macro="" textlink="">
-            <xdr:nvSpPr>
-              <xdr:cNvPr id="41" name="Oval 40"/>
-              <xdr:cNvSpPr/>
-            </xdr:nvSpPr>
-            <xdr:spPr>
-              <a:xfrm>
-                <a:off x="8238970" y="9493250"/>
-                <a:ext cx="111280" cy="109527"/>
-              </a:xfrm>
-              <a:prstGeom prst="ellipse">
-                <a:avLst/>
-              </a:prstGeom>
-              <a:grpFill/>
-              <a:ln>
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-              </a:ln>
-            </xdr:spPr>
-            <xdr:style>
-              <a:lnRef idx="2">
-                <a:schemeClr val="accent1">
-                  <a:shade val="50000"/>
-                </a:schemeClr>
-              </a:lnRef>
-              <a:fillRef idx="1">
-                <a:schemeClr val="accent1"/>
-              </a:fillRef>
-              <a:effectRef idx="0">
-                <a:schemeClr val="accent1"/>
-              </a:effectRef>
-              <a:fontRef idx="minor">
-                <a:schemeClr val="lt1"/>
-              </a:fontRef>
-            </xdr:style>
-            <xdr:txBody>
-              <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr algn="l"/>
-                <a:endParaRPr lang="en-US" sz="1100"/>
-              </a:p>
-            </xdr:txBody>
-          </xdr:sp>
-          <xdr:sp macro="" textlink="">
-            <xdr:nvSpPr>
-              <xdr:cNvPr id="42" name="Oval 41"/>
-              <xdr:cNvSpPr/>
-            </xdr:nvSpPr>
-            <xdr:spPr>
-              <a:xfrm>
-                <a:off x="8343291" y="9493250"/>
-                <a:ext cx="111280" cy="109527"/>
-              </a:xfrm>
-              <a:prstGeom prst="ellipse">
-                <a:avLst/>
-              </a:prstGeom>
-              <a:grpFill/>
-              <a:ln>
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-              </a:ln>
-            </xdr:spPr>
-            <xdr:style>
-              <a:lnRef idx="2">
-                <a:schemeClr val="accent1">
-                  <a:shade val="50000"/>
-                </a:schemeClr>
-              </a:lnRef>
-              <a:fillRef idx="1">
-                <a:schemeClr val="accent1"/>
-              </a:fillRef>
-              <a:effectRef idx="0">
-                <a:schemeClr val="accent1"/>
-              </a:effectRef>
-              <a:fontRef idx="minor">
-                <a:schemeClr val="lt1"/>
-              </a:fontRef>
-            </xdr:style>
-            <xdr:txBody>
-              <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr algn="l"/>
-                <a:endParaRPr lang="en-US" sz="1100"/>
-              </a:p>
-            </xdr:txBody>
-          </xdr:sp>
-        </xdr:grpSp>
-        <xdr:grpSp>
-          <xdr:nvGrpSpPr>
-            <xdr:cNvPr id="35" name="Group 34"/>
-            <xdr:cNvGrpSpPr/>
-          </xdr:nvGrpSpPr>
-          <xdr:grpSpPr>
-            <a:xfrm>
-              <a:off x="8238970" y="9704918"/>
-              <a:ext cx="215601" cy="109527"/>
-              <a:chOff x="8238970" y="9493250"/>
-              <a:chExt cx="215601" cy="109527"/>
-            </a:xfrm>
-            <a:grpFill/>
-          </xdr:grpSpPr>
-          <xdr:sp macro="" textlink="">
-            <xdr:nvSpPr>
-              <xdr:cNvPr id="39" name="Oval 38"/>
-              <xdr:cNvSpPr/>
-            </xdr:nvSpPr>
-            <xdr:spPr>
-              <a:xfrm>
-                <a:off x="8238970" y="9493250"/>
-                <a:ext cx="111280" cy="109527"/>
-              </a:xfrm>
-              <a:prstGeom prst="ellipse">
-                <a:avLst/>
-              </a:prstGeom>
-              <a:grpFill/>
-              <a:ln>
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-              </a:ln>
-            </xdr:spPr>
-            <xdr:style>
-              <a:lnRef idx="2">
-                <a:schemeClr val="accent1">
-                  <a:shade val="50000"/>
-                </a:schemeClr>
-              </a:lnRef>
-              <a:fillRef idx="1">
-                <a:schemeClr val="accent1"/>
-              </a:fillRef>
-              <a:effectRef idx="0">
-                <a:schemeClr val="accent1"/>
-              </a:effectRef>
-              <a:fontRef idx="minor">
-                <a:schemeClr val="lt1"/>
-              </a:fontRef>
-            </xdr:style>
-            <xdr:txBody>
-              <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr algn="l"/>
-                <a:endParaRPr lang="en-US" sz="1100"/>
-              </a:p>
-            </xdr:txBody>
-          </xdr:sp>
-          <xdr:sp macro="" textlink="">
-            <xdr:nvSpPr>
-              <xdr:cNvPr id="40" name="Oval 39"/>
-              <xdr:cNvSpPr/>
-            </xdr:nvSpPr>
-            <xdr:spPr>
-              <a:xfrm>
-                <a:off x="8343291" y="9493250"/>
-                <a:ext cx="111280" cy="109527"/>
-              </a:xfrm>
-              <a:prstGeom prst="ellipse">
-                <a:avLst/>
-              </a:prstGeom>
-              <a:grpFill/>
-              <a:ln>
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-              </a:ln>
-            </xdr:spPr>
-            <xdr:style>
-              <a:lnRef idx="2">
-                <a:schemeClr val="accent1">
-                  <a:shade val="50000"/>
-                </a:schemeClr>
-              </a:lnRef>
-              <a:fillRef idx="1">
-                <a:schemeClr val="accent1"/>
-              </a:fillRef>
-              <a:effectRef idx="0">
-                <a:schemeClr val="accent1"/>
-              </a:effectRef>
-              <a:fontRef idx="minor">
-                <a:schemeClr val="lt1"/>
-              </a:fontRef>
-            </xdr:style>
-            <xdr:txBody>
-              <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr algn="l"/>
-                <a:endParaRPr lang="en-US" sz="1100"/>
-              </a:p>
-            </xdr:txBody>
-          </xdr:sp>
-        </xdr:grpSp>
-        <xdr:grpSp>
-          <xdr:nvGrpSpPr>
-            <xdr:cNvPr id="36" name="Group 35"/>
-            <xdr:cNvGrpSpPr/>
-          </xdr:nvGrpSpPr>
-          <xdr:grpSpPr>
-            <a:xfrm>
-              <a:off x="8238970" y="9810751"/>
-              <a:ext cx="215601" cy="109527"/>
-              <a:chOff x="8238970" y="9493250"/>
-              <a:chExt cx="215601" cy="109527"/>
-            </a:xfrm>
-            <a:grpFill/>
-          </xdr:grpSpPr>
-          <xdr:sp macro="" textlink="">
-            <xdr:nvSpPr>
-              <xdr:cNvPr id="37" name="Oval 36"/>
-              <xdr:cNvSpPr/>
-            </xdr:nvSpPr>
-            <xdr:spPr>
-              <a:xfrm>
-                <a:off x="8238970" y="9493250"/>
-                <a:ext cx="111280" cy="109527"/>
-              </a:xfrm>
-              <a:prstGeom prst="ellipse">
-                <a:avLst/>
-              </a:prstGeom>
-              <a:grpFill/>
-              <a:ln>
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-              </a:ln>
-            </xdr:spPr>
-            <xdr:style>
-              <a:lnRef idx="2">
-                <a:schemeClr val="accent1">
-                  <a:shade val="50000"/>
-                </a:schemeClr>
-              </a:lnRef>
-              <a:fillRef idx="1">
-                <a:schemeClr val="accent1"/>
-              </a:fillRef>
-              <a:effectRef idx="0">
-                <a:schemeClr val="accent1"/>
-              </a:effectRef>
-              <a:fontRef idx="minor">
-                <a:schemeClr val="lt1"/>
-              </a:fontRef>
-            </xdr:style>
-            <xdr:txBody>
-              <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr algn="l"/>
-                <a:endParaRPr lang="en-US" sz="1100"/>
-              </a:p>
-            </xdr:txBody>
-          </xdr:sp>
-          <xdr:sp macro="" textlink="">
-            <xdr:nvSpPr>
-              <xdr:cNvPr id="38" name="Oval 37"/>
-              <xdr:cNvSpPr/>
-            </xdr:nvSpPr>
-            <xdr:spPr>
-              <a:xfrm>
-                <a:off x="8343291" y="9493250"/>
-                <a:ext cx="111280" cy="109527"/>
-              </a:xfrm>
-              <a:prstGeom prst="ellipse">
-                <a:avLst/>
-              </a:prstGeom>
-              <a:grpFill/>
-              <a:ln>
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-              </a:ln>
-            </xdr:spPr>
-            <xdr:style>
-              <a:lnRef idx="2">
-                <a:schemeClr val="accent1">
-                  <a:shade val="50000"/>
-                </a:schemeClr>
-              </a:lnRef>
-              <a:fillRef idx="1">
-                <a:schemeClr val="accent1"/>
-              </a:fillRef>
-              <a:effectRef idx="0">
-                <a:schemeClr val="accent1"/>
-              </a:effectRef>
-              <a:fontRef idx="minor">
-                <a:schemeClr val="lt1"/>
-              </a:fontRef>
-            </xdr:style>
-            <xdr:txBody>
-              <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr algn="l"/>
-                <a:endParaRPr lang="en-US" sz="1100"/>
-              </a:p>
-            </xdr:txBody>
-          </xdr:sp>
-        </xdr:grpSp>
-      </xdr:grpSp>
-      <xdr:grpSp>
-        <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="46" name="Group 45"/>
-          <xdr:cNvGrpSpPr/>
-        </xdr:nvGrpSpPr>
-        <xdr:grpSpPr>
-          <a:xfrm>
-            <a:off x="8162997" y="11393146"/>
-            <a:ext cx="215601" cy="106431"/>
-            <a:chOff x="8238970" y="9493250"/>
-            <a:chExt cx="215601" cy="109527"/>
-          </a:xfrm>
-          <a:solidFill>
-            <a:srgbClr val="00FF00"/>
-          </a:solidFill>
-        </xdr:grpSpPr>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="56" name="Oval 55"/>
+            <xdr:cNvPr id="60" name="Oval 59"/>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="8238970" y="9493250"/>
-              <a:ext cx="111280" cy="109527"/>
+              <a:off x="8267318" y="11282021"/>
+              <a:ext cx="111280" cy="110399"/>
             </a:xfrm>
             <a:prstGeom prst="ellipse">
               <a:avLst/>
             </a:prstGeom>
-            <a:grpFill/>
+            <a:solidFill>
+              <a:srgbClr val="00FF00"/>
+            </a:solidFill>
             <a:ln>
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
@@ -2163,80 +2593,20 @@
         </xdr:sp>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="57" name="Oval 56"/>
+            <xdr:cNvPr id="61" name="Oval 60"/>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="8343291" y="9493250"/>
-              <a:ext cx="111280" cy="109527"/>
+              <a:off x="8180006" y="10948646"/>
+              <a:ext cx="111280" cy="110399"/>
             </a:xfrm>
             <a:prstGeom prst="ellipse">
               <a:avLst/>
             </a:prstGeom>
-            <a:grpFill/>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:endParaRPr lang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </xdr:grpSp>
-      <xdr:grpSp>
-        <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="47" name="Group 46"/>
-          <xdr:cNvGrpSpPr/>
-        </xdr:nvGrpSpPr>
-        <xdr:grpSpPr>
-          <a:xfrm>
-            <a:off x="8162997" y="11495855"/>
-            <a:ext cx="215601" cy="110399"/>
-            <a:chOff x="8238970" y="9493250"/>
-            <a:chExt cx="215601" cy="109527"/>
-          </a:xfrm>
-          <a:solidFill>
-            <a:srgbClr val="00FF00"/>
-          </a:solidFill>
-        </xdr:grpSpPr>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="54" name="Oval 53"/>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="8238970" y="9493250"/>
-              <a:ext cx="111280" cy="109527"/>
-            </a:xfrm>
-            <a:prstGeom prst="ellipse">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:grpFill/>
+            <a:solidFill>
+              <a:srgbClr val="00FF00"/>
+            </a:solidFill>
             <a:ln>
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
@@ -2270,80 +2640,20 @@
         </xdr:sp>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="55" name="Oval 54"/>
+            <xdr:cNvPr id="65" name="Oval 64"/>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="8343291" y="9493250"/>
-              <a:ext cx="111280" cy="109527"/>
+              <a:off x="10142266" y="12668249"/>
+              <a:ext cx="124476" cy="127722"/>
             </a:xfrm>
             <a:prstGeom prst="ellipse">
               <a:avLst/>
             </a:prstGeom>
-            <a:grpFill/>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:endParaRPr lang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </xdr:grpSp>
-      <xdr:grpSp>
-        <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="48" name="Group 47"/>
-          <xdr:cNvGrpSpPr/>
-        </xdr:nvGrpSpPr>
-        <xdr:grpSpPr>
-          <a:xfrm>
-            <a:off x="8162997" y="11602532"/>
-            <a:ext cx="215601" cy="106429"/>
-            <a:chOff x="8238970" y="9493250"/>
-            <a:chExt cx="215601" cy="109527"/>
-          </a:xfrm>
-          <a:solidFill>
-            <a:srgbClr val="00FF00"/>
-          </a:solidFill>
-        </xdr:grpSpPr>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="52" name="Oval 51"/>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="8238970" y="9493250"/>
-              <a:ext cx="111280" cy="109527"/>
-            </a:xfrm>
-            <a:prstGeom prst="ellipse">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:grpFill/>
+            <a:solidFill>
+              <a:srgbClr val="CC00CC"/>
+            </a:solidFill>
             <a:ln>
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
@@ -2377,125 +2687,20 @@
         </xdr:sp>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="53" name="Oval 52"/>
+            <xdr:cNvPr id="66" name="Oval 65"/>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="8343291" y="9493250"/>
-              <a:ext cx="111280" cy="109527"/>
+              <a:off x="9364990" y="12668249"/>
+              <a:ext cx="124476" cy="127722"/>
             </a:xfrm>
             <a:prstGeom prst="ellipse">
               <a:avLst/>
             </a:prstGeom>
-            <a:grpFill/>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:endParaRPr lang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </xdr:grpSp>
-      <xdr:grpSp>
-        <xdr:nvGrpSpPr>
-          <xdr:cNvPr id="49" name="Group 48"/>
-          <xdr:cNvGrpSpPr/>
-        </xdr:nvGrpSpPr>
-        <xdr:grpSpPr>
-          <a:xfrm>
-            <a:off x="8162997" y="11705238"/>
-            <a:ext cx="215601" cy="106431"/>
-            <a:chOff x="8238970" y="9493250"/>
-            <a:chExt cx="215601" cy="109527"/>
-          </a:xfrm>
-          <a:solidFill>
-            <a:srgbClr val="00FF00"/>
-          </a:solidFill>
-        </xdr:grpSpPr>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="50" name="Oval 49"/>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="8238970" y="9493250"/>
-              <a:ext cx="111280" cy="109527"/>
-            </a:xfrm>
-            <a:prstGeom prst="ellipse">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:grpFill/>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="2">
-              <a:schemeClr val="accent1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:lnRef>
-            <a:fillRef idx="1">
-              <a:schemeClr val="accent1"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:schemeClr val="accent1"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="lt1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:endParaRPr lang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="51" name="Oval 50"/>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="8343291" y="9493250"/>
-              <a:ext cx="111280" cy="109527"/>
-            </a:xfrm>
-            <a:prstGeom prst="ellipse">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:grpFill/>
+            <a:solidFill>
+              <a:srgbClr val="FFFF00"/>
+            </a:solidFill>
             <a:ln>
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
@@ -2530,429 +2735,255 @@
       </xdr:grpSp>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="60" name="Oval 59"/>
-          <xdr:cNvSpPr/>
+          <xdr:cNvPr id="12" name="TextBox 11"/>
+          <xdr:cNvSpPr txBox="1"/>
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="8267318" y="11282021"/>
-            <a:ext cx="111280" cy="110399"/>
+            <a:off x="7111795" y="1952625"/>
+            <a:ext cx="1064459" cy="436786"/>
           </a:xfrm>
-          <a:prstGeom prst="ellipse">
+          <a:prstGeom prst="rect">
             <a:avLst/>
           </a:prstGeom>
-          <a:solidFill>
-            <a:srgbClr val="00FF00"/>
-          </a:solidFill>
-          <a:ln>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Both</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+              <a:t> Gnd Used</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+              <a:t>(Black Wires)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="14" name="Straight Arrow Connector 13"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="7929562" y="2393156"/>
+            <a:ext cx="345282" cy="797719"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="19050">
             <a:solidFill>
               <a:schemeClr val="tx1"/>
             </a:solidFill>
+            <a:tailEnd type="arrow"/>
           </a:ln>
         </xdr:spPr>
         <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
           </a:lnRef>
-          <a:fillRef idx="1">
+          <a:fillRef idx="0">
             <a:schemeClr val="accent1"/>
           </a:fillRef>
           <a:effectRef idx="0">
             <a:schemeClr val="accent1"/>
           </a:effectRef>
           <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
+            <a:schemeClr val="tx1"/>
           </a:fontRef>
         </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="en-US" sz="1100"/>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="61" name="Oval 60"/>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="58" name="Straight Arrow Connector 57"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="8180006" y="10948646"/>
-            <a:ext cx="111280" cy="110399"/>
+            <a:off x="7786687" y="2393156"/>
+            <a:ext cx="345282" cy="797719"/>
           </a:xfrm>
-          <a:prstGeom prst="ellipse">
+          <a:prstGeom prst="straightConnector1">
             <a:avLst/>
           </a:prstGeom>
-          <a:solidFill>
-            <a:srgbClr val="00FF00"/>
-          </a:solidFill>
-          <a:ln>
+          <a:ln w="19050">
             <a:solidFill>
               <a:schemeClr val="tx1"/>
             </a:solidFill>
+            <a:tailEnd type="arrow"/>
           </a:ln>
         </xdr:spPr>
         <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
           </a:lnRef>
-          <a:fillRef idx="1">
+          <a:fillRef idx="0">
             <a:schemeClr val="accent1"/>
           </a:fillRef>
           <a:effectRef idx="0">
             <a:schemeClr val="accent1"/>
           </a:effectRef>
           <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="59" name="TextBox 58"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="7155012" y="5464969"/>
+            <a:ext cx="978025" cy="436786"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
           </a:fontRef>
         </xdr:style>
         <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+            <a:spAutoFit/>
+          </a:bodyPr>
           <a:lstStyle/>
           <a:p>
-            <a:pPr algn="l"/>
-            <a:endParaRPr lang="en-US" sz="1100"/>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>Both</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+              <a:t> 5V Used</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+              <a:t>(Red Wires)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100" b="1"/>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="63" name="Straight Arrow Connector 62"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="8084344" y="5191125"/>
+            <a:ext cx="166687" cy="226219"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:tailEnd type="arrow"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="64" name="Straight Arrow Connector 63"/>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipV="1">
+            <a:off x="7917656" y="5143502"/>
+            <a:ext cx="238126" cy="285748"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="19050">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:tailEnd type="arrow"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
     </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>515732</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>154781</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1064459" cy="436786"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="TextBox 11"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6909388" y="1952625"/>
-          <a:ext cx="1064459" cy="436786"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>Both</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
-            <a:t> Gnd Used</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
-            <a:t>(Black Wires)</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>309562</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>59531</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>654844</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="14" name="Straight Arrow Connector 13"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7727156" y="2393156"/>
-          <a:ext cx="345282" cy="797719"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="19050">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>166687</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>59531</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>511969</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="58" name="Straight Arrow Connector 57"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7584281" y="2393156"/>
-          <a:ext cx="345282" cy="797719"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="19050">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>558949</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>83344</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="978025" cy="436786"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="59" name="TextBox 58"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6952605" y="5464969"/>
-          <a:ext cx="978025" cy="436786"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>Both</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
-            <a:t> 5V Used</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
-            <a:t>(Red Wires)</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>464344</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>631031</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>35719</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="63" name="Straight Arrow Connector 62"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="7881938" y="5191125"/>
-          <a:ext cx="166687" cy="226219"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="19050">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>297656</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>119064</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>535782</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="64" name="Straight Arrow Connector 63"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="7715250" y="5143502"/>
-          <a:ext cx="238126" cy="285748"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="19050">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3247,8 +3278,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:K105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="C17" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.28515625" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -3257,10 +3288,11 @@
     <col min="2" max="2" width="14.42578125" style="4" customWidth="1"/>
     <col min="3" max="3" width="29" style="4" customWidth="1"/>
     <col min="4" max="4" width="21" style="4" customWidth="1"/>
-    <col min="5" max="5" width="28" style="5" customWidth="1"/>
+    <col min="5" max="5" width="31" style="5" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" style="5" customWidth="1"/>
     <col min="7" max="7" width="26.5703125" style="4" customWidth="1"/>
-    <col min="8" max="16384" width="10.28515625" style="4"/>
+    <col min="8" max="8" width="13.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.28515625" style="4"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:6" ht="15" x14ac:dyDescent="0.25">
@@ -3560,6 +3592,12 @@
       <c r="D26" s="2" t="s">
         <v>167</v>
       </c>
+      <c r="E26" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" s="2">
@@ -4595,7 +4633,7 @@
       </c>
       <c r="E105" s="6">
         <f>COUNTA(E4:E103)</f>
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tuning Mode via TapeEnable switch
</commit_message>
<xml_diff>
--- a/PolysixKeyAssigner/KeyAssignerPinMap - Arduino Mega 2560.xlsx
+++ b/PolysixKeyAssigner/KeyAssignerPinMap - Arduino Mega 2560.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="205">
   <si>
     <t>Pin Number</t>
   </si>
@@ -625,6 +625,15 @@
   </si>
   <si>
     <t>AudioIn (Analog Comparator)</t>
+  </si>
+  <si>
+    <t>Switch Tape Enable (Tuning Mode)</t>
+  </si>
+  <si>
+    <t>Input (No Pullup)</t>
+  </si>
+  <si>
+    <t>5V normal, 0V when active</t>
   </si>
 </sst>
 </file>
@@ -762,8 +771,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="7447918" y="2057949"/>
-          <a:ext cx="5976742" cy="4045296"/>
+          <a:off x="7449139" y="1972468"/>
+          <a:ext cx="5968194" cy="3865787"/>
           <a:chOff x="7111795" y="1952625"/>
           <a:chExt cx="5757850" cy="3949130"/>
         </a:xfrm>
@@ -3278,8 +3287,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:K105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C17" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="E74" sqref="E74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.28515625" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -4309,7 +4318,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:7" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B73" s="2">
         <v>20</v>
       </c>
@@ -4318,6 +4327,15 @@
       </c>
       <c r="D73" s="2" t="s">
         <v>17</v>
+      </c>
+      <c r="E73" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="F73" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="G73" s="4" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="74" spans="2:7" ht="28.5" x14ac:dyDescent="0.25">
@@ -4633,7 +4651,7 @@
       </c>
       <c r="E105" s="6">
         <f>COUNTA(E4:E103)</f>
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
KeyAssigner: first ribbon control
</commit_message>
<xml_diff>
--- a/PolysixKeyAssigner/KeyAssignerPinMap - Arduino Mega 2560.xlsx
+++ b/PolysixKeyAssigner/KeyAssignerPinMap - Arduino Mega 2560.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="207">
   <si>
     <t>Pin Number</t>
   </si>
@@ -634,6 +634,12 @@
   </si>
   <si>
     <t>5V normal, 0V when active</t>
+  </si>
+  <si>
+    <t>Ribbon Wiper</t>
+  </si>
+  <si>
+    <t>black wire</t>
   </si>
 </sst>
 </file>
@@ -771,8 +777,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="7449139" y="1972468"/>
-          <a:ext cx="5968194" cy="3865787"/>
+          <a:off x="7452314" y="2035968"/>
+          <a:ext cx="5965019" cy="3999137"/>
           <a:chOff x="7111795" y="1952625"/>
           <a:chExt cx="5757850" cy="3949130"/>
         </a:xfrm>
@@ -2995,6 +3001,68 @@
     </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>478422</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>79494</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="67" name="Oval 66"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9753600" y="3057525"/>
+          <a:ext cx="116472" cy="108069"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="00FF00"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3287,8 +3355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:K105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="E74" sqref="E74"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.28515625" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -3304,7 +3372,7 @@
     <col min="9" max="16384" width="10.28515625" style="4"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" ht="15" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -3321,7 +3389,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>97</v>
       </c>
@@ -3332,7 +3400,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>96</v>
       </c>
@@ -3343,7 +3411,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>95</v>
       </c>
@@ -3354,7 +3422,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
         <v>94</v>
       </c>
@@ -3365,7 +3433,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
         <v>93</v>
       </c>
@@ -3376,7 +3444,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
         <v>92</v>
       </c>
@@ -3387,7 +3455,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
         <v>91</v>
       </c>
@@ -3398,7 +3466,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
         <v>90</v>
       </c>
@@ -3408,8 +3476,17 @@
       <c r="D11" s="2" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E11" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
         <v>89</v>
       </c>
@@ -3420,7 +3497,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
         <v>88</v>
       </c>
@@ -3431,7 +3508,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="2">
         <v>87</v>
       </c>
@@ -3442,7 +3519,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="2">
         <v>86</v>
       </c>
@@ -3453,7 +3530,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="2">
         <v>85</v>
       </c>
@@ -4651,7 +4728,7 @@
       </c>
       <c r="E105" s="6">
         <f>COUNTA(E4:E103)</f>
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
KeyAssigner: continuous pitch works!
</commit_message>
<xml_diff>
--- a/PolysixKeyAssigner/KeyAssignerPinMap - Arduino Mega 2560.xlsx
+++ b/PolysixKeyAssigner/KeyAssignerPinMap - Arduino Mega 2560.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="210">
   <si>
     <t>Pin Number</t>
   </si>
@@ -640,6 +640,15 @@
   </si>
   <si>
     <t>black wire</t>
+  </si>
+  <si>
+    <t>Ribbon Ref (to AREF)</t>
+  </si>
+  <si>
+    <t>Yellow to wire to AREF</t>
+  </si>
+  <si>
+    <t>From A6 (AREF is internally 35K to gnd)</t>
   </si>
 </sst>
 </file>
@@ -707,7 +716,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -729,6 +738,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -777,8 +792,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="7452314" y="2035968"/>
-          <a:ext cx="5965019" cy="3999137"/>
+          <a:off x="7449139" y="2051843"/>
+          <a:ext cx="5952319" cy="4032475"/>
           <a:chOff x="7111795" y="1952625"/>
           <a:chExt cx="5757850" cy="3949130"/>
         </a:xfrm>
@@ -3063,6 +3078,130 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>468809</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>147777</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>585281</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>74871</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="68" name="Oval 67"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9864941" y="3027689"/>
+          <a:ext cx="116472" cy="106388"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="00FF00"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>99015</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>41321</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>215487</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>147709</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="69" name="Oval 68"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11775544" y="5083968"/>
+          <a:ext cx="116472" cy="106388"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="00FF00"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3355,8 +3494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:K105"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.28515625" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -3465,6 +3604,15 @@
       <c r="D10" s="2" t="s">
         <v>178</v>
       </c>
+      <c r="E10" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
@@ -3585,6 +3733,9 @@
       <c r="D20" s="2" t="s">
         <v>113</v>
       </c>
+      <c r="E20" s="9" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" s="2">
@@ -4728,7 +4879,7 @@
       </c>
       <c r="E105" s="6">
         <f>COUNTA(E4:E103)</f>
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>